<commit_message>
Update Part4 Part4_Questions data
</commit_message>
<xml_diff>
--- a/crawlstudy4/part4/Part4_Questions.xlsx
+++ b/crawlstudy4/part4/Part4_Questions.xlsx
@@ -451,36 +451,36 @@
         <v>71</v>
       </c>
       <c r="B2" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C2" t="str">
-        <v>W-Am Hello, this is Karen Smith. I have an appointment with Dr. Miller for my annual eye exam on Tuesday. Unfortunately, I won't be able to make it. If possible, I'd like to reschedule for later in the week. If Dr. Miller is available in the afternoon, that would work better for me. I also wanted to ask about your warranty for eyeglasses. What exactly does the warranty cover? Thank you, and please call me back at 555-0110. W-Am Xin chào, đây là Karen Smith. Tôi có một cuộc hẹn với Tiến sĩ Miller để khám mắt định kỳ hàng năm của tôi vào thứ Ba. Thật không may, tôi sẽ không thể đến được. Nếu có thể, tôi muốn lên lịch lại vào cuối tuần. Nếu bác sĩ Miller có mặt vào buổi chiều, điều đó sẽ tốt hơn cho tôi. Tôi cũng muốn hỏi về bảo hành của các bạn cho kính mắt. Chính xác thì bảo hành bao gồm những gì? Cảm ơn bạn và vui lòng gọi lại cho tôi theo số 555-0110.</v>
+        <v>W-Am: Attention all listeners! Palmer’s Gym now has several locations in your area. We have everything you need to keep fit, including exercise classes and fitness instructors ready to help you! But that’s not all. Starting in April, your membership gives you access to any of our locations across the country. So if you're traveling for business or just on vacation, you won't have to skip your workout routine! Visit our Web site to see a map of all the Palmer’s Gym locations across the nation! Dịch nghĩa: W-Am: Xin hãy chú ý tất cả mọi người! Phòng tập thể dục Palmer hiện có một số địa điểm trong khu vực của bạn. Chúng tôi có mọi thứ bạn cần để giữ dáng, bao gồm các lớp tập thể dục và huấn luyện viên thể dục sẵn sàng giúp bạn! Nhưng đó chưa phải là tất cả. Bắt đầu từ tháng Tư, tư cách thành viên của bạn sẽ cho phép bạn đến bất kỳ địa điểm nào của chúng tôi trên toàn quốc. Vì vậy, nếu bạn đang đi công tác hoặc chỉ trong kỳ nghỉ, bạn sẽ không phải bỏ qua lịch tập luyện của mình! Ghé thăm trang web của chúng tôi để xem bản đồ của tất cả các địa điểm phòng tập thể dục Palmer trên toàn quốc!</v>
       </c>
       <c r="D2" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói có khả năng đang gọi đến loại hình doanh nghiệp nào?
-A. Một tiệm làm tóc
-B. Một công ty bảo hiểm
-C. Một đại lý ô tô
-D. Một phòng khám mắt</v>
+Loại hình kinh doanh nào đang được quảng cáo?
+A. Chợ nông sản.
+B. Một trung tâm thể dục.
+C. Phòng khám y tế.
+D. Một cửa hàng bán đồ thể thao.</v>
       </c>
       <c r="E2" t="str">
-        <v>What kind of business is the speaker most likely calling?</v>
+        <v>What type of business is being advertised?</v>
       </c>
       <c r="F2" t="str">
-        <v>A hair salon</v>
+        <v>A farmers market.</v>
       </c>
       <c r="G2" t="str">
-        <v>An insurance company</v>
+        <v>A fitness center.</v>
       </c>
       <c r="H2" t="str">
-        <v>A car dealership</v>
+        <v>A medical clinic.</v>
       </c>
       <c r="I2" t="str">
-        <v>An eye doctor's office</v>
+        <v>A sporting goods store.</v>
       </c>
       <c r="J2" t="str">
-        <v>Câu hỏi về danh tính, địa điểm, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="3" xml:space="preserve">
@@ -488,36 +488,36 @@
         <v>72</v>
       </c>
       <c r="B3" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="C3" t="str">
-        <v>W-Am Hello, this is Karen Smith. I have an appointment with Dr. Miller for my annual eye exam on Tuesday. Unfortunately, I won't be able to make it. If possible, I'd like to reschedule for later in the week. If Dr. Miller is available in the afternoon, that would work better for me. I also wanted to ask about your warranty for eyeglasses. What exactly does the warranty cover? Thank you, and please call me back at 555-0110. W-Am Xin chào, đây là Karen Smith. Tôi có một cuộc hẹn với Tiến sĩ Miller để khám mắt định kỳ hàng năm của tôi vào thứ Ba. Thật không may, tôi sẽ không thể đến được. Nếu có thể, tôi muốn lên lịch lại vào cuối tuần. Nếu bác sĩ Miller có mặt vào buổi chiều, điều đó sẽ tốt hơn cho tôi. Tôi cũng muốn hỏi về bảo hành của các bạn cho kính mắt. Chính xác thì bảo hành bao gồm những gì? Cảm ơn bạn và vui lòng gọi lại cho tôi theo số 555-0110.</v>
+        <v>W-Am: Attention all listeners! Palmer’s Gym now has several locations in your area. We have everything you need to keep fit, including exercise classes and fitness instructors ready to help you! But that’s not all. Starting in April, your membership gives you access to any of our locations across the country. So if you're traveling for business or just on vacation, you won't have to skip your workout routine! Visit our Web site to see a map of all the Palmer’s Gym locations across the nation! Dịch nghĩa: W-Am: Xin hãy chú ý tất cả mọi người! Phòng tập thể dục Palmer hiện có một số địa điểm trong khu vực của bạn. Chúng tôi có mọi thứ bạn cần để giữ dáng, bao gồm các lớp tập thể dục và huấn luyện viên thể dục sẵn sàng giúp bạn! Nhưng đó chưa phải là tất cả. Bắt đầu từ tháng Tư, tư cách thành viên của bạn sẽ cho phép bạn đến bất kỳ địa điểm nào của chúng tôi trên toàn quốc. Vì vậy, nếu bạn đang đi công tác hoặc chỉ trong kỳ nghỉ, bạn sẽ không phải bỏ qua lịch tập luyện của mình! Ghé thăm trang web của chúng tôi để xem bản đồ của tất cả các địa điểm phòng tập thể dục Palmer trên toàn quốc!</v>
       </c>
       <c r="D3" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói nói gì về cuộc hẹn của cô ấy?
-A. Nó quá xa.
-B. Nó cần phải được lên lịch lại.
-C. Nó quá đắt.
-D. Nó phải cùng với với một người khác.</v>
+Người nghe sẽ có thể làm gì bắt đầu từ tháng Tư?
+A. Sử dụng nhiều địa điểm.
+B. Dùng thử mẫu miễn phí.
+C. Gặp chuyên gia dinh dưỡng.
+D. Tham gia một cuộc thi.</v>
       </c>
       <c r="E3" t="str">
-        <v>What does the speaker say about her appointment?</v>
+        <v>What will the listeners be able to do starting in April?</v>
       </c>
       <c r="F3" t="str">
-        <v>It is too far away.</v>
+        <v>Use multiple locations.</v>
       </c>
       <c r="G3" t="str">
-        <v>It needs to be rescheduled.</v>
+        <v>Try free samples.</v>
       </c>
       <c r="H3" t="str">
-        <v>It is too expensive.</v>
+        <v>Meet with a nutritionist.</v>
       </c>
       <c r="I3" t="str">
-        <v>It should be with a different a person.</v>
+        <v>Enter a contest.</v>
       </c>
       <c r="J3" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -525,36 +525,36 @@
         <v>73</v>
       </c>
       <c r="B4" t="str">
-        <v>C</v>
+        <v>D</v>
       </c>
       <c r="C4" t="str">
-        <v>W-Am Hello, this is Karen Smith. I have an appointment with Dr. Miller for my annual eye exam on Tuesday. Unfortunately, I won't be able to make it. If possible, I'd like to reschedule for later in the week. If Dr. Miller is available in the afternoon, that would work better for me. I also wanted to ask about your warranty for eyeglasses. What exactly does the warranty cover? Thank you, and please call me back at 555-0110. W-Am Xin chào, đây là Karen Smith. Tôi có một cuộc hẹn với Tiến sĩ Miller để khám mắt định kỳ hàng năm của tôi vào thứ Ba. Thật không may, tôi sẽ không thể đến được. Nếu có thể, tôi muốn lên lịch lại vào cuối tuần. Nếu bác sĩ Miller có mặt vào buổi chiều, điều đó sẽ tốt hơn cho tôi. Tôi cũng muốn hỏi về bảo hành của các bạn cho kính mắt. Chính xác thì bảo hành bao gồm những gì? Cảm ơn bạn và vui lòng gọi lại cho tôi theo số 555-0110.</v>
+        <v>W-Am: Attention all listeners! Palmer’s Gym now has several locations in your area. We have everything you need to keep fit, including exercise classes and fitness instructors ready to help you! But that’s not all. Starting in April, your membership gives you access to any of our locations across the country. So if you're traveling for business or just on vacation, you won't have to skip your workout routine! Visit our Web site to see a map of all the Palmer’s Gym locations across the nation! Dịch nghĩa: W-Am: Xin hãy chú ý tất cả mọi người! Phòng tập thể dục Palmer hiện có một số địa điểm trong khu vực của bạn. Chúng tôi có mọi thứ bạn cần để giữ dáng, bao gồm các lớp tập thể dục và huấn luyện viên thể dục sẵn sàng giúp bạn! Nhưng đó chưa phải là tất cả. Bắt đầu từ tháng Tư, tư cách thành viên của bạn sẽ cho phép bạn đến bất kỳ địa điểm nào của chúng tôi trên toàn quốc. Vì vậy, nếu bạn đang đi công tác hoặc chỉ trong kỳ nghỉ, bạn sẽ không phải bỏ qua lịch tập luyện của mình! Ghé thăm trang web của chúng tôi để xem bản đồ của tất cả các địa điểm phòng tập thể dục Palmer trên toàn quốc!</v>
       </c>
       <c r="D4" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói muốn tìm hiểu thêm về điều gì?
-A. Phương thức thanh toán
-B. Tùy chọn giao hàng
-C. Bảo hành
-D. Việc làm đang tuyển</v>
+Tại sao người nói mời người nghe vào thăm một trang Web?
+A. Để viết bình luận.
+B. Để đăng ký một lớp học.
+C. Để kiểm tra một chính sách.
+D. Để nhìn vào bản đồ.</v>
       </c>
       <c r="E4" t="str">
-        <v>What is the speaker interested in learning more about?</v>
+        <v>Why does the speaker invite the listeners to visit a Web site?</v>
       </c>
       <c r="F4" t="str">
-        <v>Payment methods</v>
+        <v>To write a review.</v>
       </c>
       <c r="G4" t="str">
-        <v>Delivery options</v>
+        <v>To register for a class.</v>
       </c>
       <c r="H4" t="str">
-        <v>A warranty</v>
+        <v>To check a policy.</v>
       </c>
       <c r="I4" t="str">
-        <v>A job opening</v>
+        <v>To look at a map.</v>
       </c>
       <c r="J4" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="5" xml:space="preserve">
@@ -562,36 +562,36 @@
         <v>74</v>
       </c>
       <c r="B5" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="C5" t="str">
-        <v>M-Cn Curious about how chocolate is made? Then come visit us at Bodin's Chocolate Factory! You'll have a great time. We offer guided tours every Saturday and Sunday at our factory, located directly across from Appleton Shopping Center. During your two-hour visit, you'll observe the creation and packaging of Bodin's products. And each visitor will get their picture taken with Cheery, our adorable chocolate mascot, to take home as a souvenir. Right now, with the coupon available on our Web site, you can bring in a group of twelve or more people for half the price. Download yours today! M-Cn Tò mò về cách làm sô cô la? Thì, hãy đến thăm chúng tôi tại Nhà máy Sôcôla của Bodin's! Bạn sẽ có một khoảng thời gian tuyệt vời. Chúng tôi cung cấp các chuyến tham quan có hướng dẫn viên vào thứ Bảy và Chủ nhật hàng tuần tại nhà máy của chúng tôi, nằm ngay đối diện Trung tâm Mua sắm Appleton. Trong chuyến thăm kéo dài hai giờ, bạn sẽ quan sát quá trình tạo ra và đóng gói các sản phẩm của Bodin. Và mỗi du khách sẽ được chụp ảnh với Cheery, linh vật sô cô la đáng yêu của chúng tôi, để mang về nhà làm kỷ niệm. Ngay bây giờ, với phiếu giảm giá có sẵn trên trang Web của chúng tôi, bạn có thể mang theo một nhóm từ mười hai người trở lên với giá chỉ bằng một nửa. Tải xuống phiếu của bạn ngay hôm nay!</v>
+        <v>W-Br: Before we end this meeting, I want to thank everyone for the extra hours you've put in getting our new line of camera accessories ready for market. Because of your willingness to work overtime, the new products will be ready in time for the trade show coming up next month in Shanghai. That's in addition to the accessories we usually display, but it shouldn’t be a problem. We've reserved a booth at the front of the exhibition hall this year, and it's a large space. Dịch nghĩa: W-Br: Trước khi chúng ta kết thúc cuộc họp này, tôi muốn cảm ơn tất cả mọi người vì đã dành thêm giờ để đưa dòng phụ kiện máy ảnh mới của chúng ta sẵn sàng ra thị trường. Vì sự sẵn sàng làm ngoài giờ của các bạn, các sản phẩm mới sẽ sẵn sàng kịp lúc cho triển lãm thương mại sắp diễn ra vào tháng tới tại Thượng Hải. Đó là sự bổ sung cho các phụ kiện chúng ta thường trưng bày, nhưng nó không phải là một vấn đề. Chúng tôi đã đặt một gian hàng ở phía trước của phòng triển lãm năm nay, và đó là một không gian rộng lớn.</v>
       </c>
       <c r="D5" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Điều gì đang được quảng cáo?
-A. Một chuyến tham quan nhà máy
-B. Một cuộc thi làm bánh
-C. Một buổi khai trương
-D. Một buổi biểu diễn nghệ thuật</v>
+Tại sao người nói cảm ơn người nghe?
+A. Để gửi ý tưởng thiết kế.
+B. Để đào tạo nhân viên mới.
+C. Để làm thêm giờ.
+D. Để đạt được chứng nhận.</v>
       </c>
       <c r="E5" t="str">
-        <v>What is being advertised?</v>
+        <v>Why does the speaker thank the listeners?</v>
       </c>
       <c r="F5" t="str">
-        <v>A factory tour</v>
+        <v>For submitting design ideas.</v>
       </c>
       <c r="G5" t="str">
-        <v>A baking competition</v>
+        <v>For training new employees.</v>
       </c>
       <c r="H5" t="str">
-        <v>A grand opening</v>
+        <v>For working overtime.</v>
       </c>
       <c r="I5" t="str">
-        <v>An art show</v>
+        <v>For earning a certification.</v>
       </c>
       <c r="J5" t="str">
-        <v>Câu hỏi về chủ đề, mục đích, Dạng bài: Advertisement - Quảng cáo</v>
+        <v/>
       </c>
     </row>
     <row r="6" xml:space="preserve">
@@ -599,36 +599,36 @@
         <v>75</v>
       </c>
       <c r="B6" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C6" t="str">
-        <v>M-Cn Curious about how chocolate is made? Then come visit us at Bodin's Chocolate Factory! You'll have a great time. We offer guided tours every Saturday and Sunday at our factory, located directly across from Appleton Shopping Center. During your two-hour visit, you'll observe the creation and packaging of Bodin's products. And each visitor will get their picture taken with Cheery, our adorable chocolate mascot, to take home as a souvenir. Right now, with the coupon available on our Web site, you can bring in a group of twelve or more people for half the price. Download yours today! M-Cn Tò mò về cách làm sô cô la? Thì, hãy đến thăm chúng tôi tại Nhà máy Sôcôla của Bodin's! Bạn sẽ có một khoảng thời gian tuyệt vời. Chúng tôi cung cấp các chuyến tham quan có hướng dẫn viên vào thứ Bảy và Chủ nhật hàng tuần tại nhà máy của chúng tôi, nằm ngay đối diện Trung tâm Mua sắm Appleton. Trong chuyến thăm kéo dài hai giờ, bạn sẽ quan sát quá trình tạo ra và đóng gói các sản phẩm của Bodin. Và mỗi du khách sẽ được chụp ảnh với Cheery, linh vật sô cô la đáng yêu của chúng tôi, để mang về nhà làm kỷ niệm. Ngay bây giờ, với phiếu giảm giá có sẵn trên trang Web của chúng tôi, bạn có thể mang theo một nhóm từ mười hai người trở lên với giá chỉ bằng một nửa. Tải xuống phiếu của bạn ngay hôm nay!</v>
+        <v>W-Br: Before we end this meeting, I want to thank everyone for the extra hours you've put in getting our new line of camera accessories ready for market. Because of your willingness to work overtime, the new products will be ready in time for the trade show coming up next month in Shanghai. That's in addition to the accessories we usually display, but it shouldn’t be a problem. We've reserved a booth at the front of the exhibition hall this year, and it's a large space. Dịch nghĩa: W-Br: Trước khi chúng ta kết thúc cuộc họp này, tôi muốn cảm ơn tất cả mọi người vì đã dành thêm giờ để đưa dòng phụ kiện máy ảnh mới của chúng ta sẵn sàng ra thị trường. Vì sự sẵn sàng làm ngoài giờ của các bạn, các sản phẩm mới sẽ sẵn sàng kịp lúc cho triển lãm thương mại sắp diễn ra vào tháng tới tại Thượng Hải. Đó là sự bổ sung cho các phụ kiện chúng ta thường trưng bày, nhưng nó không phải là một vấn đề. Chúng tôi đã đặt một gian hàng ở phía trước của phòng triển lãm năm nay, và đó là một không gian rộng lớn.</v>
       </c>
       <c r="D6" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người tham gia sẽ nhận được gì?
-A. Một tấm áp phích
-B. Một chiếc cốc quảng cáo
-C. Một chiếc áo thun công ty
-D. Một bức ảnh</v>
+Theo diễn giả, những gì được lên kế hoạch cho tháng tới?
+A. Lễ kỷ niệm nghỉ hưu
+B. Triển lãm thương mại
+C. Một chuyến tham quan nhà máy
+D. Khai trương cửa hàng</v>
       </c>
       <c r="E6" t="str">
-        <v>What will participants receive?</v>
+        <v>According to the speaker, what is scheduled for next month?</v>
       </c>
       <c r="F6" t="str">
-        <v>A poster</v>
+        <v>A retirement celebration</v>
       </c>
       <c r="G6" t="str">
-        <v>A promotional mug</v>
+        <v>A trade show</v>
       </c>
       <c r="H6" t="str">
-        <v>A company T-shirt</v>
+        <v>A factory tour</v>
       </c>
       <c r="I6" t="str">
-        <v>A photograph</v>
+        <v>A store opening</v>
       </c>
       <c r="J6" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Advertisement - Quảng cáo</v>
+        <v/>
       </c>
     </row>
     <row r="7" xml:space="preserve">
@@ -636,36 +636,36 @@
         <v>76</v>
       </c>
       <c r="B7" t="str">
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="C7" t="str">
-        <v>M-Cn Curious about how chocolate is made? Then come visit us at Bodin's Chocolate Factory! You'll have a great time. We offer guided tours every Saturday and Sunday at our factory, located directly across from Appleton Shopping Center. During your two-hour visit, you'll observe the creation and packaging of Bodin's products. And each visitor will get their picture taken with Cheery, our adorable chocolate mascot, to take home as a souvenir. Right now, with the coupon available on our Web site, you can bring in a group of twelve or more people for half the price. Download yours today! M-Cn Tò mò về cách làm sô cô la? Thì, hãy đến thăm chúng tôi tại Nhà máy Sôcôla của Bodin's! Bạn sẽ có một khoảng thời gian tuyệt vời. Chúng tôi cung cấp các chuyến tham quan có hướng dẫn viên vào thứ Bảy và Chủ nhật hàng tuần tại nhà máy của chúng tôi, nằm ngay đối diện Trung tâm Mua sắm Appleton. Trong chuyến thăm kéo dài hai giờ, bạn sẽ quan sát quá trình tạo ra và đóng gói các sản phẩm của Bodin. Và mỗi du khách sẽ được chụp ảnh với Cheery, linh vật sô cô la đáng yêu của chúng tôi, để mang về nhà làm kỷ niệm. Ngay bây giờ, với phiếu giảm giá có sẵn trên trang Web của chúng tôi, bạn có thể mang theo một nhóm từ mười hai người trở lên với giá chỉ bằng một nửa. Tải xuống phiếu của bạn ngay hôm nay!</v>
+        <v>W-Br: Before we end this meeting, I want to thank everyone for the extra hours you've put in getting our new line of camera accessories ready for market. Because of your willingness to work overtime, the new products will be ready in time for the trade show coming up next month in Shanghai. That's in addition to the accessories we usually display, but it shouldn’t be a problem. We've reserved a booth at the front of the exhibition hall this year, and it's a large space. Dịch nghĩa: W-Br: Trước khi chúng ta kết thúc cuộc họp này, tôi muốn cảm ơn tất cả mọi người vì đã dành thêm giờ để đưa dòng phụ kiện máy ảnh mới của chúng ta sẵn sàng ra thị trường. Vì sự sẵn sàng làm ngoài giờ của các bạn, các sản phẩm mới sẽ sẵn sàng kịp lúc cho triển lãm thương mại sắp diễn ra vào tháng tới tại Thượng Hải. Đó là sự bổ sung cho các phụ kiện chúng ta thường trưng bày, nhưng nó không phải là một vấn đề. Chúng tôi đã đặt một gian hàng ở phía trước của phòng triển lãm năm nay, và đó là một không gian rộng lớn.</v>
       </c>
       <c r="D7" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nghe có thể làm gì trên một trang Web?
-A. Tìm một công thức
-B. Điền vào mẫu đăng ký
-C. Xem danh sách sản phẩm
-D. Tải xuống phiếu giảm giá</v>
+Người nói ám chỉ điều gì khi nói "đó là một không gian rộng lớn"?
+A. Có chỗ để trưng bày hàng hóa mới.
+B. Dự kiến ​​lượng người tham dự sẽ cao.
+C. Đại lộ quá đắt.
+D. Không có đủ nhân sự cho một sự kiện.</v>
       </c>
       <c r="E7" t="str">
-        <v>What can the listeners do on a Web site?</v>
+        <v>What does the speaker imply when she says, "it's a large space"?</v>
       </c>
       <c r="F7" t="str">
-        <v>Find a recipe</v>
+        <v>There is room to display new merchandise.</v>
       </c>
       <c r="G7" t="str">
-        <v>Fill out an entry form</v>
+        <v>High attendance is anticipated.</v>
       </c>
       <c r="H7" t="str">
-        <v>View a product list</v>
+        <v>Avenue is too expensive.</v>
       </c>
       <c r="I7" t="str">
-        <v>Download a coupon</v>
+        <v>There is not enough staff for an event.</v>
       </c>
       <c r="J7" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Advertisement - Quảng cáo</v>
+        <v/>
       </c>
     </row>
     <row r="8" xml:space="preserve">
@@ -673,36 +673,36 @@
         <v>77</v>
       </c>
       <c r="B8" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="C8" t="str">
-        <v>W-Br Attention, everyone. Unfortunately, we've had to stop the movie. As you've probably noticed, we're having technical difficulties with the audio. I'm very sorry about this-we take our sound quality seriously and want you to know we'll have technicians here as soon as possible to resolve this issue. As you exit, please stop by the customer service desk in the lobby to pick up two free tickets for your next movie. Again, my apologies for the inconvenience. W-Br Xin hãy chú ý, mọi người. Thật không may, chúng tôi đã phải dừng bộ phim. Như các bạn có thể đã nhận thấy, chúng tôi đang gặp sự cố kỹ thuật với âm thanh. Tôi rất tiếc về điều này - chúng tôi rất coi trọng chất lượng âm thanh của mình và muốn các bạn biết rằng chúng tôi sẽ có kỹ thuật viên ở đây sớm nhất có thể để giải quyết vấn đề này. Khi bạn ra về, vui lòng ghé lại quầy dịch vụ khách hàng ở sảnh đợi để nhận hai vé miễn phí cho bộ phim tiếp theo của các bạn. Một lần nữa, tôi xin lỗi vì sự bất tiện này.</v>
+        <v>M-Cn: Good evening. My name’s Mateo and I'll be serving you tonight. Since this is your first time here, let me tell you about our restaurant. All the vegetable products you see on the menu come from our very own vegetable garden. The owner of the café, Natasha, is a talented gardener who grows our fresh produce herself. Now, tonight we have a special entrée. It’s poached salmon, caught fresh today. It's a simple dish, served with a lemon sauce and a salad. I eat it all the time. So, while you read over the menu, can I bring you a beverage? Dịch nghĩa: M-Cn: Chào buổi tối. Tên tôi là Mateo và tôi sẽ phục vụ bạn tối nay. Vì đây là lần đầu tiên của bạn ở đây, hãy để tôi nói với bạn về nhà hàng của chúng tôi. Tất cả các sản phẩm rau bạn nhìn thấy trong thực đơn đến từ vườn rau riêng của chúng tôi. Chủ sở hữu của quán ăn, Natasha, là một người làm vườn tài năng, người tự trồng sản phẩm tươi sống của chúng tôi. Bây giờ, tối nay chúng ta có món khai vị đặc biệt. Đó là cá hồi rim, được bắt còn tươi trong hôm nay. Đó là một món ăn đơn giản, ăn kèm với nước sốt chanh và rau trộn. Tôi ăn nó mọi lúc. Vậy, trong khi bạn xem qua menu, tôi có thể mang cho bạn đồ uống không?</v>
       </c>
       <c r="D8" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Thông báo diễn ra ở đâu?
-A. Tại một nhà thi đấu thể thao
-B. Tại phòng hòa nhạc
-C. Tại bảo tàng nghệ thuật
-D. Tại rạp chiếu phim</v>
+Theo người nói, nhà hàng có gì đặc biệt?
+A. Nó có chỗ ngồi ngoài trời riêng.
+B. Nó gần đây đã được cải tạo.
+C. Nó có một vườn rau.
+D. Nó có lớp học nấu ăn hàng tuần.</v>
       </c>
       <c r="E8" t="str">
-        <v>Where does the announcement take place?</v>
+        <v>According to the speaker, what is special about the restaurant?</v>
       </c>
       <c r="F8" t="str">
-        <v>At a sports arena</v>
+        <v>It has private outdoor seating.</v>
       </c>
       <c r="G8" t="str">
-        <v>At a concert hall</v>
+        <v>It has been recently renovated.</v>
       </c>
       <c r="H8" t="str">
-        <v>At an art museum</v>
+        <v>It has a vegetable garden.</v>
       </c>
       <c r="I8" t="str">
-        <v>At a movie theater</v>
+        <v>It has weekly cooking classes.</v>
       </c>
       <c r="J8" t="str">
-        <v>Câu hỏi về danh tính, địa điểm, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="9" xml:space="preserve">
@@ -710,36 +710,36 @@
         <v>78</v>
       </c>
       <c r="B9" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="C9" t="str">
-        <v>W-Br Attention, everyone. Unfortunately, we've had to stop the movie. As you've probably noticed, we're having technical difficulties with the audio. I'm very sorry about this-we take our sound quality seriously and want you to know we'll have technicians here as soon as possible to resolve this issue. As you exit, please stop by the customer service desk in the lobby to pick up two free tickets for your next movie. Again, my apologies for the inconvenience. W-Br Xin hãy chú ý, mọi người. Thật không may, chúng tôi đã phải dừng bộ phim. Như các bạn có thể đã nhận thấy, chúng tôi đang gặp sự cố kỹ thuật với âm thanh. Tôi rất tiếc về điều này - chúng tôi rất coi trọng chất lượng âm thanh của mình và muốn các bạn biết rằng chúng tôi sẽ có kỹ thuật viên ở đây sớm nhất có thể để giải quyết vấn đề này. Khi bạn ra về, vui lòng ghé lại quầy dịch vụ khách hàng ở sảnh đợi để nhận hai vé miễn phí cho bộ phim tiếp theo của các bạn. Một lần nữa, tôi xin lỗi vì sự bất tiện này.</v>
+        <v>M-Cn: Good evening. My name’s Mateo and I'll be serving you tonight. Since this is your first time here, let me tell you about our restaurant. All the vegetable products you see on the menu come from our very own vegetable garden. The owner of the café, Natasha, is a talented gardener who grows our fresh produce herself. Now, tonight we have a special entrée. It’s poached salmon, caught fresh today. It's a simple dish, served with a lemon sauce and a salad. I eat it all the time. So, while you read over the menu, can I bring you a beverage? Dịch nghĩa: M-Cn: Chào buổi tối. Tên tôi là Mateo và tôi sẽ phục vụ bạn tối nay. Vì đây là lần đầu tiên của bạn ở đây, hãy để tôi nói với bạn về nhà hàng của chúng tôi. Tất cả các sản phẩm rau bạn nhìn thấy trong thực đơn đến từ vườn rau riêng của chúng tôi. Chủ sở hữu của quán ăn, Natasha, là một người làm vườn tài năng, người tự trồng sản phẩm tươi sống của chúng tôi. Bây giờ, tối nay chúng ta có món khai vị đặc biệt. Đó là cá hồi rim, được bắt còn tươi trong hôm nay. Đó là một món ăn đơn giản, ăn kèm với nước sốt chanh và rau trộn. Tôi ăn nó mọi lúc. Vậy, trong khi bạn xem qua menu, tôi có thể mang cho bạn đồ uống không?</v>
       </c>
       <c r="D9" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Tại sao người nói lại xin lỗi?
-A. Người thuyết trình đã bị trì hoãn.
-B. Một số đèn đã tắt.
-C. Hệ thống âm thanh bị hỏng.
-D. Một dự án xây dựng ồn ào.</v>
+Natasha là ai?
+A. Một chủ doanh nghiệp.
+B. Người trang trí nội thất.
+C. Người tổ chức sự kiện.
+D. Một nhà văn thực phẩm.</v>
       </c>
       <c r="E9" t="str">
-        <v>Why does the speaker apologize?</v>
+        <v>Who is Natasha?</v>
       </c>
       <c r="F9" t="str">
-        <v>A presenter has been delayed.</v>
+        <v>A business owner.</v>
       </c>
       <c r="G9" t="str">
-        <v>Some lights have gone out.</v>
+        <v>An interior decorator.</v>
       </c>
       <c r="H9" t="str">
-        <v>A sound system is broken.</v>
+        <v>An event organizer.</v>
       </c>
       <c r="I9" t="str">
-        <v>A construction project is noisy.</v>
+        <v>A food writer.</v>
       </c>
       <c r="J9" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="10" xml:space="preserve">
@@ -747,36 +747,36 @@
         <v>79</v>
       </c>
       <c r="B10" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C10" t="str">
-        <v>W-Br Attention, everyone. Unfortunately, we've had to stop the movie. As you've probably noticed, we're having technical difficulties with the audio. I'm very sorry about this-we take our sound quality seriously and want you to know we'll have technicians here as soon as possible to resolve this issue. As you exit, please stop by the customer service desk in the lobby to pick up two free tickets for your next movie. Again, my apologies for the inconvenience. W-Br Xin hãy chú ý, mọi người. Thật không may, chúng tôi đã phải dừng bộ phim. Như các bạn có thể đã nhận thấy, chúng tôi đang gặp sự cố kỹ thuật với âm thanh. Tôi rất tiếc về điều này - chúng tôi rất coi trọng chất lượng âm thanh của mình và muốn các bạn biết rằng chúng tôi sẽ có kỹ thuật viên ở đây sớm nhất có thể để giải quyết vấn đề này. Khi bạn ra về, vui lòng ghé lại quầy dịch vụ khách hàng ở sảnh đợi để nhận hai vé miễn phí cho bộ phim tiếp theo của các bạn. Một lần nữa, tôi xin lỗi vì sự bất tiện này.</v>
+        <v>M-Cn: Good evening. My name’s Mateo and I'll be serving you tonight. Since this is your first time here, let me tell you about our restaurant. All the vegetable products you see on the menu come from our very own vegetable garden. The owner of the café, Natasha, is a talented gardener who grows our fresh produce herself. Now, tonight we have a special entrée. It’s poached salmon, caught fresh today. It's a simple dish, served with a lemon sauce and a salad. I eat it all the time. So, while you read over the menu, can I bring you a beverage? Dịch nghĩa: M-Cn: Chào buổi tối. Tên tôi là Mateo và tôi sẽ phục vụ bạn tối nay. Vì đây là lần đầu tiên của bạn ở đây, hãy để tôi nói với bạn về nhà hàng của chúng tôi. Tất cả các sản phẩm rau bạn nhìn thấy trong thực đơn đến từ vườn rau riêng của chúng tôi. Chủ sở hữu của quán ăn, Natasha, là một người làm vườn tài năng, người tự trồng sản phẩm tươi sống của chúng tôi. Bây giờ, tối nay chúng ta có món khai vị đặc biệt. Đó là cá hồi rim, được bắt còn tươi trong hôm nay. Đó là một món ăn đơn giản, ăn kèm với nước sốt chanh và rau trộn. Tôi ăn nó mọi lúc. Vậy, trong khi bạn xem qua menu, tôi có thể mang cho bạn đồ uống không?</v>
       </c>
       <c r="D10" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói cung cấp cho người nghe điều gì?
-A. Một mặt hàng khuyến mại
-B. Một phiếu đậu xe
-C. Đồ ăn nhẹ giảm giá
-D. Vé miễn phí</v>
+Tại sao người nói nói, “Tôi ăn nó mọi lúc”?
+A. Anh ấy muốn ăn thứ gì đó khác.
+B. Anh ấy đang giới thiệu một món ăn.
+C. Anh ấy biết các thành phần.
+D. Anh ấy hiểu một món ăn là phổ biến.</v>
       </c>
       <c r="E10" t="str">
-        <v>What does the speaker offer the listeners?</v>
+        <v>Why does the speaker say, "I eat it all the time"?</v>
       </c>
       <c r="F10" t="str">
-        <v>A promotional item</v>
+        <v>He wants to eat something different.</v>
       </c>
       <c r="G10" t="str">
-        <v>A parking voucher</v>
+        <v>He is recommending a dish.</v>
       </c>
       <c r="H10" t="str">
-        <v>Discounted snacks</v>
+        <v>He knows the ingredients.</v>
       </c>
       <c r="I10" t="str">
-        <v>Free tickets</v>
+        <v>He understands a dish is popular.</v>
       </c>
       <c r="J10" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="11" xml:space="preserve">
@@ -784,36 +784,36 @@
         <v>80</v>
       </c>
       <c r="B11" t="str">
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="C11" t="str">
-        <v>W-Am Welcome to Branson Tech's second annual conference on computer security. We decided to try something different to publicize the event this year. We advertised primarily through social media rather than by e-mail newsletters or on company Web sites. And over 300 people are here! The first presentations will begin in fifteen minutes. The talks will take place in different rooms throughout the building, So please be sure to check your programs for the list of topics, speakers, and locations. W-Am Chào mừng đến với hội nghị thường niên lần thứ hai của Branson Tech về bảo mật máy tính. Chúng tôi quyết định thử một cái gì đó khác biệt để công bố sự kiện năm nay. Chúng tôi đã quảng cáo chủ yếu thông qua mạng xã hội hơn là qua các bản tin e-mail hoặc trên các trang web của công ty. Và hơn 300 người đang ở đây! Các bài thuyết trình đầu tiên sẽ bắt đầu sau mười lăm phút. Các cuộc nói chuyện sẽ diễn ra tại các phòng khác nhau trong toàn bộ tòa nhà, Vì vậy hãy nhớ kiểm tra các chương trình của bạn để biết danh sách các chủ đề, diễn giả và địa điểm.</v>
+        <v>M-Au: Welcome aboard this morning’s direct flight to Toronto. We look forward to flying with you today. Unfortunately, we've run out of space in the overhead bins for larger carry-on bags. If your bag won't fit under your seat, we'll take it from you and check it. You'll be able to pick it up at the baggage claim when we land. In addition, we have several meal options for purchase today. Our standard selections are listed in the magazine in the seat pocket in front of you. If you would like to purchase a meal, please notify a flight attendant. Dịch nghĩa: M-Au: Chào mừng đến với chuyến bay sáng nay trực tiếp đến Toronto. Chúng tôi mong chờ được bay với các bạn ngày hôm nay. Thật không may, chúng tôi đã hết chỗ trong các ngăn trên cao cho các túi mang theo lớn. Nếu túi của bạn không vừa với chỗ ngồi của bạn, chúng tôi sẽ lấy nó từ bạn và kiểm tra nó. Bạn sẽ có thể nhận nó tại điểm nhận hành lý khi chúng tôi hạ cánh. Ngoài ra, chúng tôi có một vài lựa chọn bữa ăn để mua ngày hôm nay. Các lựa chọn tiêu chuẩn của chúng tôi được liệt kê trong tạp chí trong túi ghế trước mặt bạn. Nếu bạn muốn mua một bữa ăn, xin vui lòng thông báo cho tiếp viên hàng không.</v>
       </c>
       <c r="D11" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Sự kiện gì đang diễn ra?
-A. Một hội nghị công nghệ
-B. Một buổi trưng bày giới thiệu sản phẩm
-C. Một buổi gây quỹ của công ty
-D. Một hội thảo đào tạo</v>
+Thông báo diễn ra ở đâu?
+A. Trên xe buýt.
+B. Trên một chiếc phà.
+C. Trên một chuyến tàu.
+D. Trên máy bay.</v>
       </c>
       <c r="E11" t="str">
-        <v>What event is taking place?</v>
+        <v>Where is the announcement being made?</v>
       </c>
       <c r="F11" t="str">
-        <v>A technology conference</v>
+        <v>On a bus.</v>
       </c>
       <c r="G11" t="str">
-        <v>A product demonstration</v>
+        <v>On a ferry boat.</v>
       </c>
       <c r="H11" t="str">
-        <v>A company fund-raiser</v>
+        <v>On a train.</v>
       </c>
       <c r="I11" t="str">
-        <v>A training workshop</v>
+        <v>On an airplane.</v>
       </c>
       <c r="J11" t="str">
-        <v>Câu hỏi về chủ đề, mục đích, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="12" xml:space="preserve">
@@ -821,36 +821,36 @@
         <v>81</v>
       </c>
       <c r="B12" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="C12" t="str">
-        <v>W-Am Welcome to Branson Tech's second annual conference on computer security. We decided to try something different to publicize the event this year. We advertised primarily through social media rather than by e-mail newsletters or on company Web sites. And over 300 people are here! The first presentations will begin in fifteen minutes. The talks will take place in different rooms throughout the building, So please be sure to check your programs for the list of topics, speakers, and locations. W-Am Chào mừng đến với hội nghị thường niên lần thứ hai của Branson Tech về bảo mật máy tính. Chúng tôi quyết định thử một cái gì đó khác biệt để công bố sự kiện năm nay. Chúng tôi đã quảng cáo chủ yếu thông qua mạng xã hội hơn là qua các bản tin e-mail hoặc trên các trang web của công ty. Và hơn 300 người đang ở đây! Các bài thuyết trình đầu tiên sẽ bắt đầu sau mười lăm phút. Các cuộc nói chuyện sẽ diễn ra tại các phòng khác nhau trong toàn bộ tòa nhà, Vì vậy hãy nhớ kiểm tra các chương trình của bạn để biết danh sách các chủ đề, diễn giả và địa điểm.</v>
+        <v>M-Au: Welcome aboard this morning’s direct flight to Toronto. We look forward to flying with you today. Unfortunately, we've run out of space in the overhead bins for larger carry-on bags. If your bag won't fit under your seat, we'll take it from you and check it. You'll be able to pick it up at the baggage claim when we land. In addition, we have several meal options for purchase today. Our standard selections are listed in the magazine in the seat pocket in front of you. If you would like to purchase a meal, please notify a flight attendant. Dịch nghĩa: M-Au: Chào mừng đến với chuyến bay sáng nay trực tiếp đến Toronto. Chúng tôi mong chờ được bay với các bạn ngày hôm nay. Thật không may, chúng tôi đã hết chỗ trong các ngăn trên cao cho các túi mang theo lớn. Nếu túi của bạn không vừa với chỗ ngồi của bạn, chúng tôi sẽ lấy nó từ bạn và kiểm tra nó. Bạn sẽ có thể nhận nó tại điểm nhận hành lý khi chúng tôi hạ cánh. Ngoài ra, chúng tôi có một vài lựa chọn bữa ăn để mua ngày hôm nay. Các lựa chọn tiêu chuẩn của chúng tôi được liệt kê trong tạp chí trong túi ghế trước mặt bạn. Nếu bạn muốn mua một bữa ăn, xin vui lòng thông báo cho tiếp viên hàng không.</v>
       </c>
       <c r="D12" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Tại sao người nói lại nói rằng "And over 300 people are here"?
-A. Để đề xuất chuyển đến một địa điểm lớn hơn
-B. Để chỉ ra rằng một số quảng cáo đã thành công
-C. Để nhấn mạnh tầm quan trọng của việc làm việc nhanh chóng
-D. Để đề xuất thêm tình nguyện viên</v>
+Người nói đề cập đến vấn đề gì?
+A. Không còn chỗ cho túi lớn.
+B. Đã bán quá nhiều vé.
+C. Điều kiện thời tiết đã thay đổi.
+D. Một thiết bị đang được sửa chữa.</v>
       </c>
       <c r="E12" t="str">
-        <v>Why does the speaker say, "And over 300 people are here"?</v>
+        <v>What problem does the speaker mention?</v>
       </c>
       <c r="F12" t="str">
-        <v>To propose moving to a larger venue</v>
+        <v>There is no more room for large bags.</v>
       </c>
       <c r="G12" t="str">
-        <v>To indicate that some advertising was successful</v>
+        <v>Too many tickets have been sold.</v>
       </c>
       <c r="H12" t="str">
-        <v>To emphasize the importance of working quickly</v>
+        <v>Weather conditions have changed.</v>
       </c>
       <c r="I12" t="str">
-        <v>To suggest more volunteers are needed</v>
+        <v>A piece of equipment is being repaired.</v>
       </c>
       <c r="J12" t="str">
-        <v>Câu hỏi về hàm ý câu nói, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="13" xml:space="preserve">
@@ -861,33 +861,33 @@
         <v>C</v>
       </c>
       <c r="C13" t="str">
-        <v>W-Am Welcome to Branson Tech's second annual conference on computer security. We decided to try something different to publicize the event this year. We advertised primarily through social media rather than by e-mail newsletters or on company Web sites. And over 300 people are here! The first presentations will begin in fifteen minutes. The talks will take place in different rooms throughout the building, So please be sure to check your programs for the list of topics, speakers, and locations. W-Am Chào mừng đến với hội nghị thường niên lần thứ hai của Branson Tech về bảo mật máy tính. Chúng tôi quyết định thử một cái gì đó khác biệt để công bố sự kiện năm nay. Chúng tôi đã quảng cáo chủ yếu thông qua mạng xã hội hơn là qua các bản tin e-mail hoặc trên các trang web của công ty. Và hơn 300 người đang ở đây! Các bài thuyết trình đầu tiên sẽ bắt đầu sau mười lăm phút. Các cuộc nói chuyện sẽ diễn ra tại các phòng khác nhau trong toàn bộ tòa nhà, Vì vậy hãy nhớ kiểm tra các chương trình của bạn để biết danh sách các chủ đề, diễn giả và địa điểm.</v>
+        <v>M-Au: Welcome aboard this morning’s direct flight to Toronto. We look forward to flying with you today. Unfortunately, we've run out of space in the overhead bins for larger carry-on bags. If your bag won't fit under your seat, we'll take it from you and check it. You'll be able to pick it up at the baggage claim when we land. In addition, we have several meal options for purchase today. Our standard selections are listed in the magazine in the seat pocket in front of you. If you would like to purchase a meal, please notify a flight attendant. Dịch nghĩa: M-Au: Chào mừng đến với chuyến bay sáng nay trực tiếp đến Toronto. Chúng tôi mong chờ được bay với các bạn ngày hôm nay. Thật không may, chúng tôi đã hết chỗ trong các ngăn trên cao cho các túi mang theo lớn. Nếu túi của bạn không vừa với chỗ ngồi của bạn, chúng tôi sẽ lấy nó từ bạn và kiểm tra nó. Bạn sẽ có thể nhận nó tại điểm nhận hành lý khi chúng tôi hạ cánh. Ngoài ra, chúng tôi có một vài lựa chọn bữa ăn để mua ngày hôm nay. Các lựa chọn tiêu chuẩn của chúng tôi được liệt kê trong tạp chí trong túi ghế trước mặt bạn. Nếu bạn muốn mua một bữa ăn, xin vui lòng thông báo cho tiếp viên hàng không.</v>
       </c>
       <c r="D13" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói yêu cầu người nghe làm gì?
-A. Cung cấp phản hồi
-B. Tắt chuông điện thoại di động
-C. Xem lại một chương trình sự kiện
-D. Thưởng thức một số đồ uống giải khát</v>
+Theo người nói, tại sao người nghe nên nói chuyện với nhân viên?
+A. Để nhận được một voucher.
+B. Để đặt chỗ.
+C. Để mua đồ ăn.
+D. Để nhận được tai nghe miễn phí.</v>
       </c>
       <c r="E13" t="str">
-        <v>What does the speaker ask the listeners to do?</v>
+        <v>According to the speaker, why should the listeners talk with a staff member?</v>
       </c>
       <c r="F13" t="str">
-        <v>Provide feedback</v>
+        <v>To receive a voucher.</v>
       </c>
       <c r="G13" t="str">
-        <v>Silence mobile phones</v>
+        <v>To reserve a seat.</v>
       </c>
       <c r="H13" t="str">
-        <v>Review an event program</v>
+        <v>To buy some food.</v>
       </c>
       <c r="I13" t="str">
-        <v>Enjoy some refreshments</v>
+        <v>To get free headphones.</v>
       </c>
       <c r="J13" t="str">
-        <v>Câu hỏi yêu cầu, gợi ý, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="14" xml:space="preserve">
@@ -895,36 +895,36 @@
         <v>83</v>
       </c>
       <c r="B14" t="str">
-        <v>C</v>
+        <v>D</v>
       </c>
       <c r="C14" t="str">
-        <v>M-Au Welcome, everyone. On behalf of the Department of Transportation, I'd like to announce a new experimental program to reduce traffic in Greenville. Beginning in January, there will be a ten-dollar fee for each car that enters the city. There will, however, be a lower fee for people who commute to Greenville for work. They will be asked to pay five dollars rather than ten dollars. These charges are aimed at deterring drivers from coming into this very crowded area. The program will be in effect for three months. After that, we will determine if the program has decreased traffic congestion enough to continue it permanently. M-Au Chào mừng tất cả mọi người. Thay mặt Sở Giao thông vận tải, tôi muốn thông báo một chương trình thử nghiệm mới để giảm lưu lượng giao thông ở Greenville. Bắt đầu từ tháng Giêng, sẽ có một khoản phí 10 đô la cho mỗi chiếc xe hơi vào thành phố. Tuy nhiên, sẽ có mức phí thấp hơn cho những người đến Greenville để làm việc. Họ sẽ được yêu cầu trả năm đô la thay vì mười đô la. Những khoản phí này nhằm mục đích răn đe các tài xế đi vào khu vực rất đông đúc này. Chương trình sẽ có hiệu lực trong ba tháng. Sau đó, chúng tôi sẽ xác định xem chương trình đã giảm tắc nghẽn giao thông đủ để tiếp tục nó vĩnh viễn hay chưa.</v>
+        <v>W-Am: Hello. It’s Dana, one of your truck drivers. I'm supposed to deliver kitchen appliances to our store branches in Syracuse. I’m looking for one of the branches, and according to the list I was given, there should be a store at 33 Thistle Lane. Well, I've driven up and down the whole road, and all I see are houses. I'll deliver the appliances to the other stores on my list, but while I'm doing that, could you please get back to me with the correct address? Dịch nghĩa: W-Am: Xin chào. Đây là Dana, một trong những tài xế xe tải của bạn. Tôi lẽ ra phải chuyển các dụng cụ nhà bếp cho các chi nhánh cửa hàng của chúng ta ở Syracuse. Tôi đang tìm kiếm một trong những chi nhánh, và theo danh sách tôi được cung cấp, phải có một cửa hàng tại số 33 Thistle Lane. Chà, tôi đã lái xe lên xuống cả con đường, và tất cả những gì tôi thấy là những ngôi nhà. Tôi sẽ giao các dụng cụ cho các cửa hàng khác trong danh sách của mình, nhưng trong khi tôi đang làm điều đó, bạn có thể vui lòng liên hệ lại với tôi với địa chỉ chính xác không?</v>
       </c>
       <c r="D14" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Mục đích của kế hoạch là gì?
-A. Để hỗ trợ các doanh nghiệp địa phương
-B. Để quảng bá du lịch
-C. Để giảm tắc nghẽn giao thông
-D. Để giảm chi tiêu chính phủ</v>
+Ai là người nói?
+A. Một nhân viên sửa chữa.
+B. Nhân viên cửa hàng.
+C. Một công nhân nhà máy.
+D. Một tài xế xe tải.</v>
       </c>
       <c r="E14" t="str">
-        <v>What is the purpose of the plan?</v>
+        <v>Who is the speaker?</v>
       </c>
       <c r="F14" t="str">
-        <v>To support local businesses</v>
+        <v>A repair person.</v>
       </c>
       <c r="G14" t="str">
-        <v>To promote tourism</v>
+        <v>A store clerk.</v>
       </c>
       <c r="H14" t="str">
-        <v>To decrease traffic</v>
+        <v>A factory worker.</v>
       </c>
       <c r="I14" t="str">
-        <v>To reduce government spending</v>
+        <v>A truck driver.</v>
       </c>
       <c r="J14" t="str">
-        <v>Câu hỏi về chủ đề, mục đích, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="15" xml:space="preserve">
@@ -932,36 +932,36 @@
         <v>84</v>
       </c>
       <c r="B15" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="C15" t="str">
-        <v>M-Au Welcome, everyone. On behalf of the Department of Transportation, I'd like to announce a new experimental program to reduce traffic in Greenville. Beginning in January, there will be a ten-dollar fee for each car that enters the city. There will, however, be a lower fee for people who commute to Greenville for work. They will be asked to pay five dollars rather than ten dollars. These charges are aimed at deterring drivers from coming into this very crowded area. The program will be in effect for three months. After that, we will determine if the program has decreased traffic congestion enough to continue it permanently. M-Au Chào mừng tất cả mọi người. Thay mặt Sở Giao thông vận tải, tôi muốn thông báo một chương trình thử nghiệm mới để giảm lưu lượng giao thông ở Greenville. Bắt đầu từ tháng Giêng, sẽ có một khoản phí 10 đô la cho mỗi chiếc xe hơi vào thành phố. Tuy nhiên, sẽ có mức phí thấp hơn cho những người đến Greenville để làm việc. Họ sẽ được yêu cầu trả năm đô la thay vì mười đô la. Những khoản phí này nhằm mục đích răn đe các tài xế đi vào khu vực rất đông đúc này. Chương trình sẽ có hiệu lực trong ba tháng. Sau đó, chúng tôi sẽ xác định xem chương trình đã giảm tắc nghẽn giao thông đủ để tiếp tục nó vĩnh viễn hay chưa.</v>
+        <v>W-Am: Hello. It’s Dana, one of your truck drivers. I'm supposed to deliver kitchen appliances to our store branches in Syracuse. I’m looking for one of the branches, and according to the list I was given, there should be a store at 33 Thistle Lane. Well, I've driven up and down the whole road, and all I see are houses. I'll deliver the appliances to the other stores on my list, but while I'm doing that, could you please get back to me with the correct address? Dịch nghĩa: W-Am: Xin chào. Đây là Dana, một trong những tài xế xe tải của bạn. Tôi lẽ ra phải chuyển các dụng cụ nhà bếp cho các chi nhánh cửa hàng của chúng ta ở Syracuse. Tôi đang tìm kiếm một trong những chi nhánh, và theo danh sách tôi được cung cấp, phải có một cửa hàng tại số 33 Thistle Lane. Chà, tôi đã lái xe lên xuống cả con đường, và tất cả những gì tôi thấy là những ngôi nhà. Tôi sẽ giao các dụng cụ cho các cửa hàng khác trong danh sách của mình, nhưng trong khi tôi đang làm điều đó, bạn có thể vui lòng liên hệ lại với tôi với địa chỉ chính xác không?</v>
       </c>
       <c r="D15" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói cho rằng ai sẽ được giảm giá?
-A. Người đi làm
-B. Người cao tuổi
-C. Học sinh
-D. Cán bộ thành phố</v>
+Công ty bán gì?
+A. Đồ nội thất gia đình.
+B. Dụng cụ nhà bếp.
+C. Thực phẩm đóng gói.
+D. Thiết bị xây dựng.</v>
       </c>
       <c r="E15" t="str">
-        <v>Who does the speaker say will receive a discount?</v>
+        <v>What does the company sell?</v>
       </c>
       <c r="F15" t="str">
-        <v>Commuters</v>
+        <v>Household furniture.</v>
       </c>
       <c r="G15" t="str">
-        <v>Senior citizens</v>
+        <v>Kitchen appliances.</v>
       </c>
       <c r="H15" t="str">
-        <v>Students</v>
+        <v>Packaged foods.</v>
       </c>
       <c r="I15" t="str">
-        <v>City officials</v>
+        <v>Construction equipment.</v>
       </c>
       <c r="J15" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="16" xml:space="preserve">
@@ -969,36 +969,36 @@
         <v>85</v>
       </c>
       <c r="B16" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C16" t="str">
-        <v>M-Au Welcome, everyone. On behalf of the Department of Transportation, I'd like to announce a new experimental program to reduce traffic in Greenville. Beginning in January, there will be a ten-dollar fee for each car that enters the city. There will, however, be a lower fee for people who commute to Greenville for work. They will be asked to pay five dollars rather than ten dollars. These charges are aimed at deterring drivers from coming into this very crowded area. The program will be in effect for three months. After that, we will determine if the program has decreased traffic congestion enough to continue it permanently. M-Au Chào mừng tất cả mọi người. Thay mặt Sở Giao thông vận tải, tôi muốn thông báo một chương trình thử nghiệm mới để giảm lưu lượng giao thông ở Greenville. Bắt đầu từ tháng Giêng, sẽ có một khoản phí 10 đô la cho mỗi chiếc xe hơi vào thành phố. Tuy nhiên, sẽ có mức phí thấp hơn cho những người đến Greenville để làm việc. Họ sẽ được yêu cầu trả năm đô la thay vì mười đô la. Những khoản phí này nhằm mục đích răn đe các tài xế đi vào khu vực rất đông đúc này. Chương trình sẽ có hiệu lực trong ba tháng. Sau đó, chúng tôi sẽ xác định xem chương trình đã giảm tắc nghẽn giao thông đủ để tiếp tục nó vĩnh viễn hay chưa.</v>
+        <v>W-Am: Hello. It’s Dana, one of your truck drivers. I'm supposed to deliver kitchen appliances to our store branches in Syracuse. I’m looking for one of the branches, and according to the list I was given, there should be a store at 33 Thistle Lane. Well, I've driven up and down the whole road, and all I see are houses. I'll deliver the appliances to the other stores on my list, but while I'm doing that, could you please get back to me with the correct address? Dịch nghĩa: W-Am: Xin chào. Đây là Dana, một trong những tài xế xe tải của bạn. Tôi lẽ ra phải chuyển các dụng cụ nhà bếp cho các chi nhánh cửa hàng của chúng ta ở Syracuse. Tôi đang tìm kiếm một trong những chi nhánh, và theo danh sách tôi được cung cấp, phải có một cửa hàng tại số 33 Thistle Lane. Chà, tôi đã lái xe lên xuống cả con đường, và tất cả những gì tôi thấy là những ngôi nhà. Tôi sẽ giao các dụng cụ cho các cửa hàng khác trong danh sách của mình, nhưng trong khi tôi đang làm điều đó, bạn có thể vui lòng liên hệ lại với tôi với địa chỉ chính xác không?</v>
       </c>
       <c r="D16" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Điều gì sẽ xảy ra sau ba tháng?
-A. Một cuộc khảo sát sẽ được phân phát.
-B. Một giám đốc mới sẽ tiếp quản.
-C. Một tuyến xe buýt sẽ được thêm vào.
-D. Một cuộc đánh giá chương trình sẽ diễn ra.</v>
+Người nói ám chỉ điều gì khi nói, "tất cả những gì tôi thấy là những ngôi nhà"?
+A. Cô ấy lo ngại về một số quy định.
+B. Cô ấy nghĩ đã có một lỗi sai.
+C. Đơn xin vay đã được hoàn thành.
+D. Kế hoạch phát triển không thể được phê duyệt.</v>
       </c>
       <c r="E16" t="str">
-        <v>What will happen after three months?</v>
+        <v>What does the speaker imply when she says, "all I see are houses"?</v>
       </c>
       <c r="F16" t="str">
-        <v>A survey will be distributed.</v>
+        <v>She is concerned about some regulations.</v>
       </c>
       <c r="G16" t="str">
-        <v>A new director will take over.</v>
+        <v>She thinks a mistake has been made.</v>
       </c>
       <c r="H16" t="str">
-        <v>A bus line will be added.</v>
+        <v>A loan application has been completed.</v>
       </c>
       <c r="I16" t="str">
-        <v>A program evaluation will take place.</v>
+        <v>A development plan cannot be approved.</v>
       </c>
       <c r="J16" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Announcement - Thông báo</v>
+        <v/>
       </c>
     </row>
     <row r="17" xml:space="preserve">
@@ -1006,36 +1006,36 @@
         <v>86</v>
       </c>
       <c r="B17" t="str">
-        <v>B</v>
+        <v>D</v>
       </c>
       <c r="C17" t="str">
-        <v>W-Br Thanks for tuning in to Music Today on Radio 49. First, a reminder that the Classical Music Festival is this weekend. Radio 49 is giving listeners a chance to win a pair of tickets by entering a contest. And tickets are almost sold out. Just go to our Web site and tell us what you enjoy most on our station, and we'll pick a winner at random. This year is the tenth anniversary of the event, which was founded by a famous classical musician, Umesh Gupta. On tomorrow morning's program, Mr. Gupta will be here for an interview about the history of the festival. Be sure to join us for that. W-Br Cảm ơn bạn đã theo dõi Music Today trên Radio 49. Đầu tiên, xin nhắc lại rằng Lễ hội Âm nhạc Cổ điển diễn ra vào cuối tuần này. Radio 49 đang mang đến cho thính giả cơ hội giành được một cặp vé bằng cách tham gia một cuộc thi. Và vé gần như đã được bán hết. Chỉ cần truy cập trang web của chúng tôi và cho chúng tôi biết bạn thích gì nhất trên đài của chúng tôi, và chúng tôi sẽ chọn ngẫu nhiên một người chiến thắng. Năm nay là kỷ niệm 10 năm sự kiện được thành lập bởi một nhạc sĩ cổ điển nổi tiếng, Umesh Gupta. Trong chương trình sáng mai, ông Gupta sẽ có mặt ở đây để phỏng vấn về lịch sử của lễ hội. Hãy chắc chắn tham gia với chúng tôi vì điều đó.</v>
+        <v>M-Cn: Good afternoon. My name is Lawrence Wilson, and I'll be conducting the training on how to use our company’s new scheduling software-Spark Schedule. The reason we chose this particular software is because it makes it easy for you to schedule meetings with people in different time zones. That way we can conduct business with our increasing number of clients all over the world. And best of all, there’s a mobile phone application that you can download for free. This will allow you to check your schedule from any location. Dịch nghĩa: M-Cn: Chào buổi chiều. Tên tôi là Lawrence Wilson và tôi sẽ tiến hành tập huấn về cách sử dụng phần mềm lập lịch trình mới của công ty chúng tôi - Spark Schedule. Lý do chúng tôi chọn phần mềm cụ thể này là vì nó giúp bạn dễ dàng lên lịch các cuộc họp với mọi người ở các múi giờ khác nhau. Bằng cách đó, chúng ta có thể tiến hành công việc với số lượng khách hàng ngày càng tăng trên toàn thế giới. Và điều tuyệt nhất là, có một ứng dụng trên điện thoại di động mà bạn có thể tải xuống miễn phí. Điều này sẽ cho phép bạn kiểm tra lịch trình của bạn từ bất kỳ vị trí nào.</v>
       </c>
       <c r="D17" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói đang thảo luận về sự kiện gì?
-A. Một cuộc thi đấu thể thao
-B. Một lễ hội âm nhạc
-C. Một buổi trình diễn nấu ăn
-D. Một vở kịch mang tính lịch sử</v>
+Bài nói chủ yếu nói về điều gì?
+A. Một mẫu điện thoại di động.
+B. Một hệ thống an ninh văn phòng.
+C. Dịch vụ Internet tốc độ cao.
+D. Phần mềm lập kế hoạch kinh doanh.</v>
       </c>
       <c r="E17" t="str">
-        <v>What event is the speaker discussing?</v>
+        <v>What is the talk mainly about?</v>
       </c>
       <c r="F17" t="str">
-        <v>A sports competition</v>
+        <v>A mobile phone model.</v>
       </c>
       <c r="G17" t="str">
-        <v>A music festival</v>
+        <v>An office security system.</v>
       </c>
       <c r="H17" t="str">
-        <v>A cooking demonstration</v>
+        <v>High-speed Internet service.</v>
       </c>
       <c r="I17" t="str">
-        <v>A historical play</v>
+        <v>Business scheduling software.</v>
       </c>
       <c r="J17" t="str">
-        <v>Câu hỏi về chủ đề, mục đích, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="18" xml:space="preserve">
@@ -1046,33 +1046,33 @@
         <v>A</v>
       </c>
       <c r="C18" t="str">
-        <v>W-Br Thanks for tuning in to Music Today on Radio 49. First, a reminder that the Classical Music Festival is this weekend. Radio 49 is giving listeners a chance to win a pair of tickets by entering a contest. And tickets are almost sold out. Just go to our Web site and tell us what you enjoy most on our station, and we'll pick a winner at random. This year is the tenth anniversary of the event, which was founded by a famous classical musician, Umesh Gupta. On tomorrow morning's program, Mr. Gupta will be here for an interview about the history of the festival. Be sure to join us for that. W-Br Cảm ơn bạn đã theo dõi Music Today trên Radio 49. Đầu tiên, xin nhắc lại rằng Lễ hội Âm nhạc Cổ điển diễn ra vào cuối tuần này. Radio 49 đang mang đến cho thính giả cơ hội giành được một cặp vé bằng cách tham gia một cuộc thi. Và vé gần như đã được bán hết. Chỉ cần truy cập trang web của chúng tôi và cho chúng tôi biết bạn thích gì nhất trên đài của chúng tôi, và chúng tôi sẽ chọn ngẫu nhiên một người chiến thắng. Năm nay là kỷ niệm 10 năm sự kiện được thành lập bởi một nhạc sĩ cổ điển nổi tiếng, Umesh Gupta. Trong chương trình sáng mai, ông Gupta sẽ có mặt ở đây để phỏng vấn về lịch sử của lễ hội. Hãy chắc chắn tham gia với chúng tôi vì điều đó.</v>
+        <v>M-Cn: Good afternoon. My name is Lawrence Wilson, and I'll be conducting the training on how to use our company’s new scheduling software-Spark Schedule. The reason we chose this particular software is because it makes it easy for you to schedule meetings with people in different time zones. That way we can conduct business with our increasing number of clients all over the world. And best of all, there’s a mobile phone application that you can download for free. This will allow you to check your schedule from any location. Dịch nghĩa: M-Cn: Chào buổi chiều. Tên tôi là Lawrence Wilson và tôi sẽ tiến hành tập huấn về cách sử dụng phần mềm lập lịch trình mới của công ty chúng tôi - Spark Schedule. Lý do chúng tôi chọn phần mềm cụ thể này là vì nó giúp bạn dễ dàng lên lịch các cuộc họp với mọi người ở các múi giờ khác nhau. Bằng cách đó, chúng ta có thể tiến hành công việc với số lượng khách hàng ngày càng tăng trên toàn thế giới. Và điều tuyệt nhất là, có một ứng dụng trên điện thoại di động mà bạn có thể tải xuống miễn phí. Điều này sẽ cho phép bạn kiểm tra lịch trình của bạn từ bất kỳ vị trí nào.</v>
       </c>
       <c r="D18" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Tại sao người nói lại nói rằng "tickets are almost sold out"?
-A. Để khuyến khích người nghe tham gia một cuộc thi
-B. Để đề nghị người nghe đến sớm
-C. Để khiếu nại rằng không gian sự kiện quá nhỏ
-D. Để khen ngợi kết quả của một kế hoạch tiếp thị</v>
+Tại sao công ty lại chọn sản phẩm này?
+A. Nó giúp việc sắp xếp các cuộc họp trở nên dễ dàng.
+B. Nó có giá hợp lý.
+C. Nó có tính năng bảo mật tốt.
+D. Nó đã nhận được những đánh giá tích cực.</v>
       </c>
       <c r="E18" t="str">
-        <v>Why does the speaker say, "tickets are almost sold out"?</v>
+        <v>Why did the company choose the product?</v>
       </c>
       <c r="F18" t="str">
-        <v>To encourage the listeners to enter a contest</v>
+        <v>It makes arranging meetings easy.</v>
       </c>
       <c r="G18" t="str">
-        <v>To suggest that the listeners arrive early</v>
+        <v>It is reasonably priced.</v>
       </c>
       <c r="H18" t="str">
-        <v>To complain that an event space is too small</v>
+        <v>It has good security features.</v>
       </c>
       <c r="I18" t="str">
-        <v>To praise the results of a marketing plan</v>
+        <v>It has received positive reviews.</v>
       </c>
       <c r="J18" t="str">
-        <v>Câu hỏi về hàm ý câu nói, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="19" xml:space="preserve">
@@ -1083,33 +1083,33 @@
         <v>C</v>
       </c>
       <c r="C19" t="str">
-        <v>W-Br Thanks for tuning in to Music Today on Radio 49. First, a reminder that the Classical Music Festival is this weekend. Radio 49 is giving listeners a chance to win a pair of tickets by entering a contest. And tickets are almost sold out. Just go to our Web site and tell us what you enjoy most on our station, and we'll pick a winner at random. This year is the tenth anniversary of the event, which was founded by a famous classical musician, Umesh Gupta. On tomorrow morning's program, Mr. Gupta will be here for an interview about the history of the festival. Be sure to join us for that. W-Br Cảm ơn bạn đã theo dõi Music Today trên Radio 49. Đầu tiên, xin nhắc lại rằng Lễ hội Âm nhạc Cổ điển diễn ra vào cuối tuần này. Radio 49 đang mang đến cho thính giả cơ hội giành được một cặp vé bằng cách tham gia một cuộc thi. Và vé gần như đã được bán hết. Chỉ cần truy cập trang web của chúng tôi và cho chúng tôi biết bạn thích gì nhất trên đài của chúng tôi, và chúng tôi sẽ chọn ngẫu nhiên một người chiến thắng. Năm nay là kỷ niệm 10 năm sự kiện được thành lập bởi một nhạc sĩ cổ điển nổi tiếng, Umesh Gupta. Trong chương trình sáng mai, ông Gupta sẽ có mặt ở đây để phỏng vấn về lịch sử của lễ hội. Hãy chắc chắn tham gia với chúng tôi vì điều đó.</v>
+        <v>M-Cn: Good afternoon. My name is Lawrence Wilson, and I'll be conducting the training on how to use our company’s new scheduling software-Spark Schedule. The reason we chose this particular software is because it makes it easy for you to schedule meetings with people in different time zones. That way we can conduct business with our increasing number of clients all over the world. And best of all, there’s a mobile phone application that you can download for free. This will allow you to check your schedule from any location. Dịch nghĩa: M-Cn: Chào buổi chiều. Tên tôi là Lawrence Wilson và tôi sẽ tiến hành tập huấn về cách sử dụng phần mềm lập lịch trình mới của công ty chúng tôi - Spark Schedule. Lý do chúng tôi chọn phần mềm cụ thể này là vì nó giúp bạn dễ dàng lên lịch các cuộc họp với mọi người ở các múi giờ khác nhau. Bằng cách đó, chúng ta có thể tiến hành công việc với số lượng khách hàng ngày càng tăng trên toàn thế giới. Và điều tuyệt nhất là, có một ứng dụng trên điện thoại di động mà bạn có thể tải xuống miễn phí. Điều này sẽ cho phép bạn kiểm tra lịch trình của bạn từ bất kỳ vị trí nào.</v>
       </c>
       <c r="D19" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Điều gì sẽ xảy ra vào sáng mai?
-A. Một địa điểm mới sẽ được mở.
-B. Người chiến thắng giải thưởng sẽ được công bố.
-C. Một cuộc phỏng vấn sẽ diễn ra.
-D. Một đoạn video sẽ được quay.</v>
+Người nói nói gì đi kèm với sản phẩm?
+A. Nâng cấp hàng năm.
+B. Đảm bảo hoàn lại tiền.
+C. Một ứng dụng điện thoại di động.
+D. Đường dây trợ giúp dịch vụ khách hàng.</v>
       </c>
       <c r="E19" t="str">
-        <v>What will happen tomorrow morning?</v>
+        <v>What does the speaker say is offered with the product?</v>
       </c>
       <c r="F19" t="str">
-        <v>A new venue will open.</v>
+        <v>An annual upgrade.</v>
       </c>
       <c r="G19" t="str">
-        <v>A prize winner will be announced.</v>
+        <v>A money-back guarantee.</v>
       </c>
       <c r="H19" t="str">
-        <v>An interview will take place.</v>
+        <v>A mobile phone application.</v>
       </c>
       <c r="I19" t="str">
-        <v>A video will be filmed.</v>
+        <v>A customer-service help line.</v>
       </c>
       <c r="J19" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="20" xml:space="preserve">
@@ -1117,36 +1117,36 @@
         <v>89</v>
       </c>
       <c r="B20" t="str">
-        <v>C</v>
+        <v>D</v>
       </c>
       <c r="C20" t="str">
-        <v>W-Am Thank you for visiting our booth here at the trade fair. We're so excited to show you our new patio furniture. You're probably familiar with our wooden outdoor tables and chairs, and we want you to know that we've expanded that line to include plastic furniture. This furniture is very durable. It can withstand any kind of weather and it needs no maintenance. I'm going to hand out a sample of the plastic material we use. Please pass it around after you've had a chance to look at it. W-Am Cảm ơn các bạn đã ghé thăm gian hàng của chúng tôi tại hội chợ thương mại. Chúng tôi rất vui mừng được giới thiệu cho các bạn đồ nội thất sân mới của chúng tôi. Có thể các bạn đã quen thuộc với những bộ bàn ghế ngoài trời bằng gỗ của chúng tôi và chúng tôi muốn các bạn biết rằng chúng tôi đã mở rộng dòng sản phẩm đó để bao gồm cả đồ nội thất bằng nhựa. Đồ nội thất này rất bền. Nó có thể chịu được mọi loại thời tiết và không cần bảo dưỡng. Tôi sẽ phát một mẫu vật liệu nhựa mà chúng tôi sử dụng. Hãy chuyển nó sau khi các bạn có cơ hội xem qua nó.</v>
+        <v>W-Br: This is Guo Lin with KDM TV News. Tonight, there’s news about the Ashworth City light-rail. Work continues on this massive construction project, but the announcement of new federal safety regulations means that major modifications must be made to the tracks. Opening day could be delayed by as much as three months. Public opinion about the railway is already divided. Some residents say they don't approve of how much money is being spent on the project, but others say it’s worth the cost. I’m here at the Fourth Street station where I'll ask a few passersby how they feel about this latest development in the project. Dịch nghĩa: W-Br: Đây là Guo Lin với bản tin KDM TV News. Tối nay là tin tức về đường sắt nội thành Ashworth City. Công việc vẫn tiếp tục trong dự án xây dựng khổng lồ này, nhưng việc thông báo các quy định an toàn mới của liên bang đồng nghĩa là phải có những sửa đổi lớn đối với đường ray. Ngày khánh thành có thể bị trì hoãn tới ba tháng. Dư luận về đường sắt đã bị chia rẽ. Một số cư dân nói rằng họ không chấp thuận số tiền chi cho dự án, nhưng những người khác nói rằng nó đáng với chi phí bỏ ra. Tôi đang ở ngay tại nhà ga Fourth Street, nơi tôi sẽ hỏi một vài người qua đường xem liệu họ cảm thấy thế nào về sự tiến triển mới nhất này trong dự án.</v>
       </c>
       <c r="D20" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói làm việc cho loại hình kinh doanh nào?
-A. Một công ty máy tính
-B. Một công ty xây dựng
-C. Một nhà sản xuất đồ nội thất
-D. Một nhà phân phối văn phòng phẩm</v>
+Người nói nói rằng điều gì đã được thông báo gần đây?
+A. Sự gia tăng nguồn tài trợ.
+B. Khai trương nhà máy.
+C. Một địa điểm mới cho một sự kiện.
+D. Một sự thay đổi trong quy định.</v>
       </c>
       <c r="E20" t="str">
-        <v>What type of business does the speaker work for?</v>
+        <v>What does the speaker say has recently been announced?</v>
       </c>
       <c r="F20" t="str">
-        <v>A computer company</v>
+        <v>An increase in funding.</v>
       </c>
       <c r="G20" t="str">
-        <v>A construction firm</v>
+        <v>A factory opening.</v>
       </c>
       <c r="H20" t="str">
-        <v>A furniture manufacturer</v>
+        <v>A new venue for an event.</v>
       </c>
       <c r="I20" t="str">
-        <v>An office-supply distributor</v>
+        <v>A change in regulations.</v>
       </c>
       <c r="J20" t="str">
-        <v>Câu hỏi về danh tính, địa điểm, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="21" xml:space="preserve">
@@ -1157,33 +1157,33 @@
         <v>B</v>
       </c>
       <c r="C21" t="str">
-        <v>W-Am Thank you for visiting our booth here at the trade fair. We're so excited to show you our new patio furniture. You're probably familiar with our wooden outdoor tables and chairs, and we want you to know that we've expanded that line to include plastic furniture. This furniture is very durable. It can withstand any kind of weather and it needs no maintenance. I'm going to hand out a sample of the plastic material we use. Please pass it around after you've had a chance to look at it. W-Am Cảm ơn các bạn đã ghé thăm gian hàng của chúng tôi tại hội chợ thương mại. Chúng tôi rất vui mừng được giới thiệu cho các bạn đồ nội thất sân mới của chúng tôi. Có thể các bạn đã quen thuộc với những bộ bàn ghế ngoài trời bằng gỗ của chúng tôi và chúng tôi muốn các bạn biết rằng chúng tôi đã mở rộng dòng sản phẩm đó để bao gồm cả đồ nội thất bằng nhựa. Đồ nội thất này rất bền. Nó có thể chịu được mọi loại thời tiết và không cần bảo dưỡng. Tôi sẽ phát một mẫu vật liệu nhựa mà chúng tôi sử dụng. Hãy chuyển nó sau khi các bạn có cơ hội xem qua nó.</v>
+        <v>W-Br: This is Guo Lin with KDM TV News. Tonight, there’s news about the Ashworth City light-rail. Work continues on this massive construction project, but the announcement of new federal safety regulations means that major modifications must be made to the tracks. Opening day could be delayed by as much as three months. Public opinion about the railway is already divided. Some residents say they don't approve of how much money is being spent on the project, but others say it’s worth the cost. I’m here at the Fourth Street station where I'll ask a few passersby how they feel about this latest development in the project. Dịch nghĩa: W-Br: Đây là Guo Lin với bản tin KDM TV News. Tối nay là tin tức về đường sắt nội thành Ashworth City. Công việc vẫn tiếp tục trong dự án xây dựng khổng lồ này, nhưng việc thông báo các quy định an toàn mới của liên bang đồng nghĩa là phải có những sửa đổi lớn đối với đường ray. Ngày khánh thành có thể bị trì hoãn tới ba tháng. Dư luận về đường sắt đã bị chia rẽ. Một số cư dân nói rằng họ không chấp thuận số tiền chi cho dự án, nhưng những người khác nói rằng nó đáng với chi phí bỏ ra. Tôi đang ở ngay tại nhà ga Fourth Street, nơi tôi sẽ hỏi một vài người qua đường xem liệu họ cảm thấy thế nào về sự tiến triển mới nhất này trong dự án.</v>
       </c>
       <c r="D21" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói cho biết ưu điểm của vật liệu mới là gì?
-A. Nó rẻ.
-B. Nó bền.
-C. Nó nhẹ.
-D. Nó có nhiều màu sắc.</v>
+Theo người nói, tại sao một số người không thích một dự án xây dựng?
+A. Bởi vì nó gây ra sự cố mất điện.
+B. Bởi vì nó tốn kém quá nhiều.
+C. Vì đường đã bị đóng.
+D. Vì tiếng ồn lớn.</v>
       </c>
       <c r="E21" t="str">
-        <v>What does the speaker say is an advantage of the new material?</v>
+        <v>According to the speaker, why do some people dislike a construction project?</v>
       </c>
       <c r="F21" t="str">
-        <v>It is inexpensive.</v>
+        <v>Because it caused a power outage.</v>
       </c>
       <c r="G21" t="str">
-        <v>It is durable.</v>
+        <v>Because it costs too much.</v>
       </c>
       <c r="H21" t="str">
-        <v>It is lightweight.</v>
+        <v>Because roads have been closed.</v>
       </c>
       <c r="I21" t="str">
-        <v>It comes in many colors.</v>
+        <v>Because of the loud noise.</v>
       </c>
       <c r="J21" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="22" xml:space="preserve">
@@ -1191,36 +1191,36 @@
         <v>91</v>
       </c>
       <c r="B22" t="str">
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="C22" t="str">
-        <v>W-Am Thank you for visiting our booth here at the trade fair. We're so excited to show you our new patio furniture. You're probably familiar with our wooden outdoor tables and chairs, and we want you to know that we've expanded that line to include plastic furniture. This furniture is very durable. It can withstand any kind of weather and it needs no maintenance. I'm going to hand out a sample of the plastic material we use. Please pass it around after you've had a chance to look at it. W-Am Cảm ơn các bạn đã ghé thăm gian hàng của chúng tôi tại hội chợ thương mại. Chúng tôi rất vui mừng được giới thiệu cho các bạn đồ nội thất sân mới của chúng tôi. Có thể các bạn đã quen thuộc với những bộ bàn ghế ngoài trời bằng gỗ của chúng tôi và chúng tôi muốn các bạn biết rằng chúng tôi đã mở rộng dòng sản phẩm đó để bao gồm cả đồ nội thất bằng nhựa. Đồ nội thất này rất bền. Nó có thể chịu được mọi loại thời tiết và không cần bảo dưỡng. Tôi sẽ phát một mẫu vật liệu nhựa mà chúng tôi sử dụng. Hãy chuyển nó sau khi các bạn có cơ hội xem qua nó.</v>
+        <v>W-Br: This is Guo Lin with KDM TV News. Tonight, there’s news about the Ashworth City light-rail. Work continues on this massive construction project, but the announcement of new federal safety regulations means that major modifications must be made to the tracks. Opening day could be delayed by as much as three months. Public opinion about the railway is already divided. Some residents say they don't approve of how much money is being spent on the project, but others say it’s worth the cost. I’m here at the Fourth Street station where I'll ask a few passersby how they feel about this latest development in the project. Dịch nghĩa: W-Br: Đây là Guo Lin với bản tin KDM TV News. Tối nay là tin tức về đường sắt nội thành Ashworth City. Công việc vẫn tiếp tục trong dự án xây dựng khổng lồ này, nhưng việc thông báo các quy định an toàn mới của liên bang đồng nghĩa là phải có những sửa đổi lớn đối với đường ray. Ngày khánh thành có thể bị trì hoãn tới ba tháng. Dư luận về đường sắt đã bị chia rẽ. Một số cư dân nói rằng họ không chấp thuận số tiền chi cho dự án, nhưng những người khác nói rằng nó đáng với chi phí bỏ ra. Tôi đang ở ngay tại nhà ga Fourth Street, nơi tôi sẽ hỏi một vài người qua đường xem liệu họ cảm thấy thế nào về sự tiến triển mới nhất này trong dự án.</v>
       </c>
       <c r="D22" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nghe sẽ làm gì tiếp theo?
-A. Đăng ký danh sách gửi thư
-B. Xem video hướng dẫn
-C. Tham gia một cuộc thi
-D. Nhìn vào một mẫu</v>
+Người nói sẽ làm gì tiếp theo?
+A. Giới thiệu nhà quảng cáo.
+B. Tham dự một cuộc họp báo.
+C. Phỏng vấn một số người.
+D. Kết thúc chương trình phát sóng.</v>
       </c>
       <c r="E22" t="str">
-        <v>What will the listeners do next?</v>
+        <v>What will the speaker do next?</v>
       </c>
       <c r="F22" t="str">
-        <v>Sign up for a mailing list</v>
+        <v>Introduce an advertiser.</v>
       </c>
       <c r="G22" t="str">
-        <v>Watch an instructional video</v>
+        <v>Attend a press conference.</v>
       </c>
       <c r="H22" t="str">
-        <v>Enter a contest</v>
+        <v>Interview some people.</v>
       </c>
       <c r="I22" t="str">
-        <v>Look at a sample</v>
+        <v>End a broadcast.</v>
       </c>
       <c r="J22" t="str">
-        <v>Câu hỏi về hành động tương lai, Dạng bài: Talk - Bài phát biểu, diễn văn</v>
+        <v/>
       </c>
     </row>
     <row r="23" xml:space="preserve">
@@ -1228,36 +1228,36 @@
         <v>92</v>
       </c>
       <c r="B23" t="str">
-        <v>B</v>
+        <v>C</v>
       </c>
       <c r="C23" t="str">
-        <v>W-Br This is Noriko, the human resources supervisor here in Albany. l'm calling about your request to transfer to our branch in Havertown... I know your commute is difficult, and it takes you over an hour to drive to this office. So I've contacted the manager at that location, and there is a need for a skilled software engineer. There are a few forms that you'll need to fill out, though, to complete the request. Now we need to talk about your work schedule to decide when you'll start at the new location. Please call me back. W-Br Đây là Noriko, giám sát nhân sự ở Albany. Tôi đang gọi về yêu cầu của bạn để chuyển đến chi nhánh của chúng tôi ở Havertown ... Tôi biết rằng đường đi làm của bạn rất khó khăn và bạn phải mất hơn một giờ lái xe đến văn phòng này. Vì vậy, tôi đã liên hệ với người quản lý tại địa điểm đó, và ở đó đang cần một kỹ sư phần mềm lành nghề. Tuy nhiên, có một số biểu mẫu mà bạn sẽ cần phải điền vào để hoàn thành yêu cầu. Bây giờ chúng ta cần nói về lịch trình làm việc của bạn để quyết định khi nào bạn sẽ bắt đầu tại địa điểm mới. Hãy gọi lại cho tôi.</v>
+        <v>M-Au: First of all, we know you have a busy schedule outside of work, so thanks for coming in to the warehouse today to work on a Saturday. OK, so we're here because this extra shipment was delivered yesterday. There are hundreds of boxes, and we have to check what's inside them and put the information into our warehouse database. Now, I'm going to assign you all to groups. Once you have your group number, go ahead and join your group members. Group leaders will tell you which boxes you'll be working on. Dịch nghĩa: M-Au: Trước hết, chúng tôi biết các bạn có một lịch trình bận rộn bên ngoài công việc, vì vậy cảm ơn các bạn đã đến nhà kho hôm nay để làm việc vào thứ bảy. Được rồi, vậy chúng ta ở đây vì hàng gửi bổ sung này đã được giao ngày hôm qua. Có hàng trăm hộp và chúng ta phải kiểm tra những gì bên trong chúng và đưa thông tin vào cơ sở dữ liệu kho của chúng ta. Bây giờ, tôi sẽ chỉ định tất cả các bạn vào các nhóm. Một khi các bạn có số nhóm của mình, hãy tiếp tục và tham gia với các thành viên trong nhóm của bạn. Trưởng nhóm sẽ cho bạn biết bạn sẽ làm việc với những hộp nào.</v>
       </c>
       <c r="D23" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói làm việc ở bộ phận nào?
-A. Phát triển sản phẩm
-B. Nhân sự
-C. Pháp lý
-D. Kế toán</v>
+Người nói cảm ơn người nghe vì điều gì?
+A. Sắp xếp lại một số tài liệu.
+B. Vệ sinh khu vực làm việc.
+C. Làm việc vào thứ bảy.
+D. Tham gia khóa đào tạo.</v>
       </c>
       <c r="E23" t="str">
-        <v>Which department does the speaker work in?</v>
+        <v>What does the speaker thank the listeners for?</v>
       </c>
       <c r="F23" t="str">
-        <v>Product Development</v>
+        <v>Reorganizing some files.</v>
       </c>
       <c r="G23" t="str">
-        <v>Human Resources</v>
+        <v>Cleaning a work area.</v>
       </c>
       <c r="H23" t="str">
-        <v>Legal</v>
+        <v>Working on a Saturday.</v>
       </c>
       <c r="I23" t="str">
-        <v>Accounting</v>
+        <v>Attending a training.</v>
       </c>
       <c r="J23" t="str">
-        <v>Câu hỏi về danh tính, địa điểm, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="24" xml:space="preserve">
@@ -1265,36 +1265,36 @@
         <v>93</v>
       </c>
       <c r="B24" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="C24" t="str">
-        <v>W-Br This is Noriko, the human resources supervisor here in Albany. l'm calling about your request to transfer to our branch in Havertown... I know your commute is difficult, and it takes you over an hour to drive to this office. So I've contacted the manager at that location, and there is a need for a skilled software engineer. There are a few forms that you'll need to fill out, though, to complete the request. Now we need to talk about your work schedule to decide when you'll start at the new location. Please call me back. W-Br Đây là Noriko, giám sát nhân sự ở Albany. Tôi đang gọi về yêu cầu của bạn để chuyển đến chi nhánh của chúng tôi ở Havertown ... Tôi biết rằng đường đi làm của bạn rất khó khăn và bạn phải mất hơn một giờ lái xe đến văn phòng này. Vì vậy, tôi đã liên hệ với người quản lý tại địa điểm đó, và ở đó đang cần một kỹ sư phần mềm lành nghề. Tuy nhiên, có một số biểu mẫu mà bạn sẽ cần phải điền vào để hoàn thành yêu cầu. Bây giờ chúng ta cần nói về lịch trình làm việc của bạn để quyết định khi nào bạn sẽ bắt đầu tại địa điểm mới. Hãy gọi lại cho tôi.</v>
+        <v>M-Au: First of all, we know you have a busy schedule outside of work, so thanks for coming in to the warehouse today to work on a Saturday. OK, so we're here because this extra shipment was delivered yesterday. There are hundreds of boxes, and we have to check what's inside them and put the information into our warehouse database. Now, I'm going to assign you all to groups. Once you have your group number, go ahead and join your group members. Group leaders will tell you which boxes you'll be working on. Dịch nghĩa: M-Au: Trước hết, chúng tôi biết các bạn có một lịch trình bận rộn bên ngoài công việc, vì vậy cảm ơn các bạn đã đến nhà kho hôm nay để làm việc vào thứ bảy. Được rồi, vậy chúng ta ở đây vì hàng gửi bổ sung này đã được giao ngày hôm qua. Có hàng trăm hộp và chúng ta phải kiểm tra những gì bên trong chúng và đưa thông tin vào cơ sở dữ liệu kho của chúng ta. Bây giờ, tôi sẽ chỉ định tất cả các bạn vào các nhóm. Một khi các bạn có số nhóm của mình, hãy tiếp tục và tham gia với các thành viên trong nhóm của bạn. Trưởng nhóm sẽ cho bạn biết bạn sẽ làm việc với những hộp nào.</v>
       </c>
       <c r="D24" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Tại sao người nói lại cho rằng “there is a need for a skilled software engineer”?
-A. Để giới thiệu nhân viên đăng ký đào tạo thêm
-B. Để chỉ ra rằng thời hạn dự án sẽ được gia hạn
-C. Để phê duyệt yêu cầu chuyển nhượng
-D. Để đề nghị tư vấn với một chuyên gia</v>
+Người nghe có khả năng làm việc ở bộ phận nào nhất?
+A. Vận chuyển và nhận hàng.
+B. Bảo trì.
+C. Bán hàng và tiếp thị.
+D. Kế toán.</v>
       </c>
       <c r="E24" t="str">
-        <v>Why does the speaker say, "there is a need for a skilled software engineer"?</v>
+        <v>In which division do the listeners most likely work?</v>
       </c>
       <c r="F24" t="str">
-        <v>To recommend an employee sign up for more training</v>
+        <v>Shipping and Receiving.</v>
       </c>
       <c r="G24" t="str">
-        <v>To indicate that a project deadline will be extended</v>
+        <v>Maintenance.</v>
       </c>
       <c r="H24" t="str">
-        <v>To approve a request to transfer</v>
+        <v>Sales and Marketing.</v>
       </c>
       <c r="I24" t="str">
-        <v>To suggest consulting with an expert</v>
+        <v>Accounting.</v>
       </c>
       <c r="J24" t="str">
-        <v>Câu hỏi về hàm ý câu nói, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="25" xml:space="preserve">
@@ -1302,36 +1302,36 @@
         <v>94</v>
       </c>
       <c r="B25" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C25" t="str">
-        <v>W-Br This is Noriko, the human resources supervisor here in Albany. l'm calling about your request to transfer to our branch in Havertown... I know your commute is difficult, and it takes you over an hour to drive to this office. So I've contacted the manager at that location, and there is a need for a skilled software engineer. There are a few forms that you'll need to fill out, though, to complete the request. Now we need to talk about your work schedule to decide when you'll start at the new location. Please call me back. W-Br Đây là Noriko, giám sát nhân sự ở Albany. Tôi đang gọi về yêu cầu của bạn để chuyển đến chi nhánh của chúng tôi ở Havertown ... Tôi biết rằng đường đi làm của bạn rất khó khăn và bạn phải mất hơn một giờ lái xe đến văn phòng này. Vì vậy, tôi đã liên hệ với người quản lý tại địa điểm đó, và ở đó đang cần một kỹ sư phần mềm lành nghề. Tuy nhiên, có một số biểu mẫu mà bạn sẽ cần phải điền vào để hoàn thành yêu cầu. Bây giờ chúng ta cần nói về lịch trình làm việc của bạn để quyết định khi nào bạn sẽ bắt đầu tại địa điểm mới. Hãy gọi lại cho tôi.</v>
+        <v>M-Au: First of all, we know you have a busy schedule outside of work, so thanks for coming in to the warehouse today to work on a Saturday. OK, so we're here because this extra shipment was delivered yesterday. There are hundreds of boxes, and we have to check what's inside them and put the information into our warehouse database. Now, I'm going to assign you all to groups. Once you have your group number, go ahead and join your group members. Group leaders will tell you which boxes you'll be working on. Dịch nghĩa: M-Au: Trước hết, chúng tôi biết các bạn có một lịch trình bận rộn bên ngoài công việc, vì vậy cảm ơn các bạn đã đến nhà kho hôm nay để làm việc vào thứ bảy. Được rồi, vậy chúng ta ở đây vì hàng gửi bổ sung này đã được giao ngày hôm qua. Có hàng trăm hộp và chúng ta phải kiểm tra những gì bên trong chúng và đưa thông tin vào cơ sở dữ liệu kho của chúng ta. Bây giờ, tôi sẽ chỉ định tất cả các bạn vào các nhóm. Một khi các bạn có số nhóm của mình, hãy tiếp tục và tham gia với các thành viên trong nhóm của bạn. Trưởng nhóm sẽ cho bạn biết bạn sẽ làm việc với những hộp nào.</v>
       </c>
       <c r="D25" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nói muốn trao đổi điều gì với người nghe?
-A. Một số kết quả bán hàng
-B. Một số phản hồi của khách hàng
-C. Cải tạo văn phòng
-D. Lịch làm việc</v>
+Người nói nói rằng anh ta sẽ cung cấp những gì?
+A. Tên tòa nhà.
+B. Số nhóm.
+C. Thay đổi lịch trình.
+D. Mật khẩu tạm thời.</v>
       </c>
       <c r="E25" t="str">
-        <v>What does the speaker want to discuss with the listener?</v>
+        <v>What does the speaker say he will provide?</v>
       </c>
       <c r="F25" t="str">
-        <v>Some sales results</v>
+        <v>A building name.</v>
       </c>
       <c r="G25" t="str">
-        <v>Some client feedback</v>
+        <v>Group numbers.</v>
       </c>
       <c r="H25" t="str">
-        <v>An office renovation</v>
+        <v>Shift schedules.</v>
       </c>
       <c r="I25" t="str">
-        <v>A work schedule</v>
+        <v>A temporary password.</v>
       </c>
       <c r="J25" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="26" xml:space="preserve">
@@ -1339,36 +1339,36 @@
         <v>95</v>
       </c>
       <c r="B26" t="str">
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="C26" t="str">
-        <v>M-Cn You're listening to Making My Company with Mark Sullivan. In each episode I invite entrepreneurs from around the world to talk about how they built their successful businesses. In celebration of our radio show's ten-year anniversary, our Web site now has all of our previously aired episodes. You can access them with the click of a button. You can even download them onto mobile devices to listen to on the go! OK, now, welcome Haru Nakamura to the show. Ms. Nakamura is excited to be here today. M-Cn Bạn đang nghe Making My Company với Mark Sullivan. Trong mỗi tập, tôi mời các doanh nhân trên khắp thế giới nói về cách họ xây dựng doanh nghiệp thành công của mình. Để kỷ niệm mười năm chương trình radio, trang Web của chúng tôi hiện có tất cả các tập đã phát sóng trước đây. Bạn có thể truy cập chúng bằng một nút bấm. Bạn thậm chí có thể tải chúng xuống thiết bị di động để nghe khi đang di chuyển! OK, bây giờ, chào mừng Haru Nakamura đến với chương trình. Cô Nakamura rất vui khi có mặt ở đây hôm nay.</v>
+        <v>W-Am: And now, an event we've all been waiting for since last year-Danville’s Annual Cook-Off. Held outside at City Park, the Cook-Off always attracts a lot of participants. Competitors prepare one dish, which they serve throughout the day. A panel of judges will select the winners based on taste, presentation, and uniqueness. This event is great fun for the whole family, and entry and food samples are free! If you're interested in participating, the contest registration form is available on the city’s Web site. Now, keep in mind we're expecting a cloudy day for this year’s event. We won't see any sunshine, so be sure to bring a jacket! Dịch nghĩa: W-Am: Và bây giờ, một sự kiện mà tất cả chúng ta đã chờ đợi từ năm ngoái - Cuộc thi nấu ăn thường niên của Cookville. Được tổ chức ngoài trời tại City Park, Cuộc thi nấu ăn luôn thu hút rất nhiều người tham gia. Các thí sinh chuẩn bị một món ăn, mà họ phục vụ trong suốt cả ngày. Một hội đồng giám khảo sẽ chọn ra những người chiến thắng dựa trên hương vị, cách trình bày và sự độc đáo. Sự kiện này là niềm vui lớn cho tất cả thành viên trong gia đình, và phí vào cổng cùng các mẫu thức ăn đều miễn phí! Nếu bạn muốn tham gia, mẫu đăng ký cuộc thi có sẵn trên trang web của thành phố. Bây giờ, hãy nhớ rằng chúng tôi đang dự kiến một ngày nhiều mây cho sự kiện năm nay. Chúng ta sẽ không thấy bất kỳ ánh nắng mặt trời nào đâu, vì vậy hãy nhớ mang theo áo khoác!</v>
       </c>
       <c r="D26" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Tại sao các vị khách được mời trên chương trình radio của diễn giả?
-A. Để thảo luận về công việc kinh doanh của họ
-B. Để nói về lịch sử địa phương
-C. Để dạy kỹ năng giao tiếp
-D. Để đưa ra lời khuyên khi đi du lịch</v>
+Sự kiện nào đang được mô tả?
+A. Một cuộc thi đấu thể thao.
+B. Một buổi lễ của chính phủ.
+C. Một lễ hội âm nhạc.
+D. Một cuộc thi nấu ăn.</v>
       </c>
       <c r="E26" t="str">
-        <v>Why are guests invited on the speaker's radio show?</v>
+        <v>What event is being described?</v>
       </c>
       <c r="F26" t="str">
-        <v>To discuss their businesses</v>
+        <v>A sports competition.</v>
       </c>
       <c r="G26" t="str">
-        <v>To talk about local history</v>
+        <v>A government ceremony.</v>
       </c>
       <c r="H26" t="str">
-        <v>To teach communication skills</v>
+        <v>A music festival.</v>
       </c>
       <c r="I26" t="str">
-        <v>To offer travel tips</v>
+        <v>A cooking contest.</v>
       </c>
       <c r="J26" t="str">
-        <v>Câu hỏi về chủ đề, mục đích, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="27" xml:space="preserve">
@@ -1379,33 +1379,33 @@
         <v>D</v>
       </c>
       <c r="C27" t="str">
-        <v>M-Cn You're listening to Making My Company with Mark Sullivan. In each episode I invite entrepreneurs from around the world to talk about how they built their successful businesses. In celebration of our radio show's ten-year anniversary, our Web site now has all of our previously aired episodes. You can access them with the click of a button. You can even download them onto mobile devices to listen to on the go! OK, now, welcome Haru Nakamura to the show. Ms. Nakamura is excited to be here today. M-Cn Bạn đang nghe Making My Company với Mark Sullivan. Trong mỗi tập, tôi mời các doanh nhân trên khắp thế giới nói về cách họ xây dựng doanh nghiệp thành công của mình. Để kỷ niệm mười năm chương trình radio, trang Web của chúng tôi hiện có tất cả các tập đã phát sóng trước đây. Bạn có thể truy cập chúng bằng một nút bấm. Bạn thậm chí có thể tải chúng xuống thiết bị di động để nghe khi đang di chuyển! OK, bây giờ, chào mừng Haru Nakamura đến với chương trình. Cô Nakamura rất vui khi có mặt ở đây hôm nay.</v>
+        <v>W-Am: And now, an event we've all been waiting for since last year-Danville’s Annual Cook-Off. Held outside at City Park, the Cook-Off always attracts a lot of participants. Competitors prepare one dish, which they serve throughout the day. A panel of judges will select the winners based on taste, presentation, and uniqueness. This event is great fun for the whole family, and entry and food samples are free! If you're interested in participating, the contest registration form is available on the city’s Web site. Now, keep in mind we're expecting a cloudy day for this year’s event. We won't see any sunshine, so be sure to bring a jacket! Dịch nghĩa: W-Am: Và bây giờ, một sự kiện mà tất cả chúng ta đã chờ đợi từ năm ngoái - Cuộc thi nấu ăn thường niên của Cookville. Được tổ chức ngoài trời tại City Park, Cuộc thi nấu ăn luôn thu hút rất nhiều người tham gia. Các thí sinh chuẩn bị một món ăn, mà họ phục vụ trong suốt cả ngày. Một hội đồng giám khảo sẽ chọn ra những người chiến thắng dựa trên hương vị, cách trình bày và sự độc đáo. Sự kiện này là niềm vui lớn cho tất cả thành viên trong gia đình, và phí vào cổng cùng các mẫu thức ăn đều miễn phí! Nếu bạn muốn tham gia, mẫu đăng ký cuộc thi có sẵn trên trang web của thành phố. Bây giờ, hãy nhớ rằng chúng tôi đang dự kiến một ngày nhiều mây cho sự kiện năm nay. Chúng ta sẽ không thấy bất kỳ ánh nắng mặt trời nào đâu, vì vậy hãy nhớ mang theo áo khoác!</v>
       </c>
       <c r="D27" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nghe có thể làm gì trên một trang Web?
-A. Xem ảnh của các vị khách nổi tiếng
-B. Đăng ký dịch vụ đặc biệt
-C. Đọc về các chương trình sắp tới
-D. Nghe các tập trước</v>
+Theo người nói, người nghe có thể tìm thấy gì trên một trang Web?
+A. Bản đồ thành phố.
+B. Danh sách các nhà cung cấp.
+C. Một video trình diễn.
+D. Đơn đăng ký.</v>
       </c>
       <c r="E27" t="str">
-        <v>What can the listeners do on a Web site?</v>
+        <v>According to the speaker, what can the listeners find on a Web site?</v>
       </c>
       <c r="F27" t="str">
-        <v>View photos of famous guests</v>
+        <v>A city map.</v>
       </c>
       <c r="G27" t="str">
-        <v>Sign up for a special service</v>
+        <v>A list of vendors.</v>
       </c>
       <c r="H27" t="str">
-        <v>Read about upcoming programs</v>
+        <v>A demonstration video.</v>
       </c>
       <c r="I27" t="str">
-        <v>Listen to previous episodes</v>
+        <v>An entry form.</v>
       </c>
       <c r="J27" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="28" xml:space="preserve">
@@ -1413,36 +1413,36 @@
         <v>97</v>
       </c>
       <c r="B28" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="C28" t="str">
-        <v>M-Cn You're listening to Making My Company with Mark Sullivan. In each episode I invite entrepreneurs from around the world to talk about how they built their successful businesses. In celebration of our radio show's ten-year anniversary, our Web site now has all of our previously aired episodes. You can access them with the click of a button. You can even download them onto mobile devices to listen to on the go! OK, now, welcome Haru Nakamura to the show. Ms. Nakamura is excited to be here today. M-Cn Bạn đang nghe Making My Company với Mark Sullivan. Trong mỗi tập, tôi mời các doanh nhân trên khắp thế giới nói về cách họ xây dựng doanh nghiệp thành công của mình. Để kỷ niệm mười năm chương trình radio, trang Web của chúng tôi hiện có tất cả các tập đã phát sóng trước đây. Bạn có thể truy cập chúng bằng một nút bấm. Bạn thậm chí có thể tải chúng xuống thiết bị di động để nghe khi đang di chuyển! OK, bây giờ, chào mừng Haru Nakamura đến với chương trình. Cô Nakamura rất vui khi có mặt ở đây hôm nay.</v>
+        <v>W-Am: And now, an event we've all been waiting for since last year-Danville’s Annual Cook-Off. Held outside at City Park, the Cook-Off always attracts a lot of participants. Competitors prepare one dish, which they serve throughout the day. A panel of judges will select the winners based on taste, presentation, and uniqueness. This event is great fun for the whole family, and entry and food samples are free! If you're interested in participating, the contest registration form is available on the city’s Web site. Now, keep in mind we're expecting a cloudy day for this year’s event. We won't see any sunshine, so be sure to bring a jacket! Dịch nghĩa: W-Am: Và bây giờ, một sự kiện mà tất cả chúng ta đã chờ đợi từ năm ngoái - Cuộc thi nấu ăn thường niên của Cookville. Được tổ chức ngoài trời tại City Park, Cuộc thi nấu ăn luôn thu hút rất nhiều người tham gia. Các thí sinh chuẩn bị một món ăn, mà họ phục vụ trong suốt cả ngày. Một hội đồng giám khảo sẽ chọn ra những người chiến thắng dựa trên hương vị, cách trình bày và sự độc đáo. Sự kiện này là niềm vui lớn cho tất cả thành viên trong gia đình, và phí vào cổng cùng các mẫu thức ăn đều miễn phí! Nếu bạn muốn tham gia, mẫu đăng ký cuộc thi có sẵn trên trang web của thành phố. Bây giờ, hãy nhớ rằng chúng tôi đang dự kiến một ngày nhiều mây cho sự kiện năm nay. Chúng ta sẽ không thấy bất kỳ ánh nắng mặt trời nào đâu, vì vậy hãy nhớ mang theo áo khoác!</v>
       </c>
       <c r="D28" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Nhìn vào hình ảnh. Tập này được phát sóng vào ngày nào?
-A. Thứ ba
-B. Thứ tư
-C. Thứ năm
-D. Thứ sáu</v>
+Nhìn vào hình. Sự kiện được tổ chức vào ngày nào?
+A. Thứ bảy.
+B. Chủ nhật.
+C. Thứ hai.
+D. Thứ ba.</v>
       </c>
       <c r="E28" t="str">
-        <v>Look at the graphic. Which day is this episode being aired?</v>
+        <v>Look at the graphic. Which day is the event being held?</v>
       </c>
       <c r="F28" t="str">
-        <v>Tuesday</v>
+        <v>Saturday.</v>
       </c>
       <c r="G28" t="str">
-        <v>Wednesday</v>
+        <v>Sunday.</v>
       </c>
       <c r="H28" t="str">
-        <v>Thursday</v>
+        <v>Monday.</v>
       </c>
       <c r="I28" t="str">
-        <v>Friday</v>
+        <v>Tuesday.</v>
       </c>
       <c r="J28" t="str">
-        <v>Câu hỏi kết hợp bảng biểu, Dạng bài: News report, Broadcast - Bản tin</v>
+        <v/>
       </c>
     </row>
     <row r="29" xml:space="preserve">
@@ -1450,36 +1450,36 @@
         <v>98</v>
       </c>
       <c r="B29" t="str">
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="C29" t="str">
-        <v>M-Au It's Akira, calling from the district manager's office. The visual merchandising team wants to make a slight change to the fall display standards that we sent you yesterday. They want to move the shirts with the vertical stripes-hang them instead of having them displayed on the shelf. We'll display some colorful accessories there instead, like scarves and ties. Also, hang all the socks on gridwall panels by the cash registers. Those sell best when people can grab them when they walk up to pay. The thicker, cold-weather socks will be shipped to you soon. You'll get an e-mail confirmation with the details when they're sent. M-Au Đây là Akira, đang gọi từ văn phòng quản lý khu. Nhóm bán hàng trực quan muốn thực hiện một chút thay đổi đối với tiêu chuẩn trưng bày mùa thu mà chúng tôi đã gửi cho bạn ngày hôm qua. Họ muốn di chuyển những chiếc áo sơ mi có sọc dọc-treo chúng thay vì để chúng được trưng bày trên giá. Thay vào đó, chúng tôi sẽ trưng bày một số phụ kiện đầy màu sắc ở đó, chẳng hạn như khăn quàng cổ và cà vạt. Ngoài ra, hãy treo tất cả những chiếc tất trên các tấm lưới của máy tính tiền. Những thứ này bán chạy nhất khi mọi người có thể lấy chúng khi họ bước đến thanh toán. Những đôi tất dày hơn, chịu được thời tiết lạnh sẽ sớm được chuyển đến cho bạn. Bạn sẽ nhận được một email xác nhận với các chi tiết khi chúng được gửi.</v>
+        <v>M-Cn: This is Seung-ho Park from Park Investors. We met last month at the Westside Technology Conference. I attended your interesting presentation and spoke to you afterward about my small investment firm. I'm calling because I'd like to hire you to discuss ways to make my company’s database more secure. I know you specialize in this type of work, and I'm hoping you'll be interested in this project. Could you please e-mail me a list of your consultant fees? Use the e-mail address on the business card I gave you. Thanks. Dịch nghĩa: M-Cn: Đây là Park Seung-ho từ Park Investors. Chúng ta đã gặp nhau vào tháng trước tại Hội nghị Công nghệ Westside. Tôi đã tham dự buổi thuyết trình thú vị của bạn và nói chuyện với bạn sau đó về hãng đầu tư nhỏ của tôi. Tôi đang gọi vì tôi muốn thuê bạn để thảo luận về các cách để làm cho cơ sở dữ liệu của công ty tôi bảo mật hơn. Tôi biết bạn chuyên môn về loại công việc này, và tôi hy vọng bạn sẽ quan tâm đến dự án này. Bạn có thể vui lòng gửi e-mail cho tôi một danh sách các khoản phí tư vấn của bạn? Sử dụng địa chỉ e-mail trên danh thiếp tôi đã đưa cho bạn. Cảm ơn.</v>
       </c>
       <c r="D29" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Nhìn vào hình ảnh. Những chiếc khăn quàng cổ và cà vạt sẽ được trưng bày ở đâu?
-A. Trên kệ 1
-B. Trên kệ 2
-C. Trên kệ 3
-D. Trên kệ 4</v>
+Mục đích của cuộc gọi là gì?
+A. Để xác nhận thời hạn.
+B. Để giải thích chính sách của công ty.
+C. Để đưa ra lời mời làm việc.
+D. Để thảo luận về một sản phẩm mới.</v>
       </c>
       <c r="E29" t="str">
-        <v>Look at the graphic. Where will the scarves and ties be displayed?</v>
+        <v>What is the purpose of the call?</v>
       </c>
       <c r="F29" t="str">
-        <v>On Shelf 1</v>
+        <v>To confirm a deadline.</v>
       </c>
       <c r="G29" t="str">
-        <v>On Shelf 2</v>
+        <v>To explain a company policy.</v>
       </c>
       <c r="H29" t="str">
-        <v>On Shelf 3</v>
+        <v>To make a job offer.</v>
       </c>
       <c r="I29" t="str">
-        <v>On Shelf 4</v>
+        <v>To discuss a new product.</v>
       </c>
       <c r="J29" t="str">
-        <v>Câu hỏi kết hợp bảng biểu, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="30" xml:space="preserve">
@@ -1487,36 +1487,36 @@
         <v>99</v>
       </c>
       <c r="B30" t="str">
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="C30" t="str">
-        <v>M-Au It's Akira, calling from the district manager's office. The visual merchandising team wants to make a slight change to the fall display standards that we sent you yesterday. They want to move the shirts with the vertical stripes-hang them instead of having them displayed on the shelf. We'll display some colorful accessories there instead, like scarves and ties. Also, hang all the socks on gridwall panels by the cash registers. Those sell best when people can grab them when they walk up to pay. The thicker, cold-weather socks will be shipped to you soon. You'll get an e-mail confirmation with the details when they're sent. M-Au Đây là Akira, đang gọi từ văn phòng quản lý khu. Nhóm bán hàng trực quan muốn thực hiện một chút thay đổi đối với tiêu chuẩn trưng bày mùa thu mà chúng tôi đã gửi cho bạn ngày hôm qua. Họ muốn di chuyển những chiếc áo sơ mi có sọc dọc-treo chúng thay vì để chúng được trưng bày trên giá. Thay vào đó, chúng tôi sẽ trưng bày một số phụ kiện đầy màu sắc ở đó, chẳng hạn như khăn quàng cổ và cà vạt. Ngoài ra, hãy treo tất cả những chiếc tất trên các tấm lưới của máy tính tiền. Những thứ này bán chạy nhất khi mọi người có thể lấy chúng khi họ bước đến thanh toán. Những đôi tất dày hơn, chịu được thời tiết lạnh sẽ sớm được chuyển đến cho bạn. Bạn sẽ nhận được một email xác nhận với các chi tiết khi chúng được gửi.</v>
+        <v>M-Cn: This is Seung-ho Park from Park Investors. We met last month at the Westside Technology Conference. I attended your interesting presentation and spoke to you afterward about my small investment firm. I'm calling because I'd like to hire you to discuss ways to make my company’s database more secure. I know you specialize in this type of work, and I'm hoping you'll be interested in this project. Could you please e-mail me a list of your consultant fees? Use the e-mail address on the business card I gave you. Thanks. Dịch nghĩa: M-Cn: Đây là Park Seung-ho từ Park Investors. Chúng ta đã gặp nhau vào tháng trước tại Hội nghị Công nghệ Westside. Tôi đã tham dự buổi thuyết trình thú vị của bạn và nói chuyện với bạn sau đó về hãng đầu tư nhỏ của tôi. Tôi đang gọi vì tôi muốn thuê bạn để thảo luận về các cách để làm cho cơ sở dữ liệu của công ty tôi bảo mật hơn. Tôi biết bạn chuyên môn về loại công việc này, và tôi hy vọng bạn sẽ quan tâm đến dự án này. Bạn có thể vui lòng gửi e-mail cho tôi một danh sách các khoản phí tư vấn của bạn? Sử dụng địa chỉ e-mail trên danh thiếp tôi đã đưa cho bạn. Cảm ơn.</v>
       </c>
       <c r="D30" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Cái gì nên được trưng bày gần máy tính tiền?
-A. Phiếu giảm giá
-B. Mũ
-C. Găng tay
-D. Tất</v>
+Nhìn vào hình. Người nói đang gọi cho ai?
+A. Carla Wynn.
+B. Jae Ho Kim.
+C. Kaori Aoki.
+D. Alex Lehmann.</v>
       </c>
       <c r="E30" t="str">
-        <v>What should be displayed near the cash registers?</v>
+        <v>Look at the graphic. Who is the speaker calling?</v>
       </c>
       <c r="F30" t="str">
-        <v>Coupons</v>
+        <v>Carla Wynn.</v>
       </c>
       <c r="G30" t="str">
-        <v>Hats</v>
+        <v>Jae-Ho Kim.</v>
       </c>
       <c r="H30" t="str">
-        <v>Gloves</v>
+        <v>Kaori Aoki.</v>
       </c>
       <c r="I30" t="str">
-        <v>Socks</v>
+        <v>Alex Lehmann.</v>
       </c>
       <c r="J30" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
     <row r="31" xml:space="preserve">
@@ -1524,36 +1524,36 @@
         <v>100</v>
       </c>
       <c r="B31" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="C31" t="str">
-        <v>M-Au It's Akira, calling from the district manager's office. The visual merchandising team wants to make a slight change to the fall display standards that we sent you yesterday. They want to move the shirts with the vertical stripes-hang them instead of having them displayed on the shelf. We'll display some colorful accessories there instead, like scarves and ties. Also, hang all the socks on gridwall panels by the cash registers. Those sell best when people can grab them when they walk up to pay. The thicker, cold-weather socks will be shipped to you soon. You'll get an e-mail confirmation with the details when they're sent. M-Au Đây là Akira, đang gọi từ văn phòng quản lý khu. Nhóm bán hàng trực quan muốn thực hiện một chút thay đổi đối với tiêu chuẩn trưng bày mùa thu mà chúng tôi đã gửi cho bạn ngày hôm qua. Họ muốn di chuyển những chiếc áo sơ mi có sọc dọc-treo chúng thay vì để chúng được trưng bày trên giá. Thay vào đó, chúng tôi sẽ trưng bày một số phụ kiện đầy màu sắc ở đó, chẳng hạn như khăn quàng cổ và cà vạt. Ngoài ra, hãy treo tất cả những chiếc tất trên các tấm lưới của máy tính tiền. Những thứ này bán chạy nhất khi mọi người có thể lấy chúng khi họ bước đến thanh toán. Những đôi tất dày hơn, chịu được thời tiết lạnh sẽ sớm được chuyển đến cho bạn. Bạn sẽ nhận được một email xác nhận với các chi tiết khi chúng được gửi.</v>
+        <v>M-Cn: This is Seung-ho Park from Park Investors. We met last month at the Westside Technology Conference. I attended your interesting presentation and spoke to you afterward about my small investment firm. I'm calling because I'd like to hire you to discuss ways to make my company’s database more secure. I know you specialize in this type of work, and I'm hoping you'll be interested in this project. Could you please e-mail me a list of your consultant fees? Use the e-mail address on the business card I gave you. Thanks. Dịch nghĩa: M-Cn: Đây là Park Seung-ho từ Park Investors. Chúng ta đã gặp nhau vào tháng trước tại Hội nghị Công nghệ Westside. Tôi đã tham dự buổi thuyết trình thú vị của bạn và nói chuyện với bạn sau đó về hãng đầu tư nhỏ của tôi. Tôi đang gọi vì tôi muốn thuê bạn để thảo luận về các cách để làm cho cơ sở dữ liệu của công ty tôi bảo mật hơn. Tôi biết bạn chuyên môn về loại công việc này, và tôi hy vọng bạn sẽ quan tâm đến dự án này. Bạn có thể vui lòng gửi e-mail cho tôi một danh sách các khoản phí tư vấn của bạn? Sử dụng địa chỉ e-mail trên danh thiếp tôi đã đưa cho bạn. Cảm ơn.</v>
       </c>
       <c r="D31" t="str" xml:space="preserve">
         <v xml:space="preserve">Dịch đáp án:
-Người nghe mong đợi nhận được gì trong e-mail?
-A. Lịch thanh toán
-B. Những bức ảnh
-C. Thông tin vận chuyển
-D. Hiển thị số đo</v>
+Người nói nhờ người nghe làm gì?
+A. Kiểm tra danh mục.
+B. Gửi thông tin phí.
+C. Gửi hành trình du lịch.
+D. Cập nhật lịch hội nghị.</v>
       </c>
       <c r="E31" t="str">
-        <v>What should the listener expect to receive in an e-mail?</v>
+        <v>What does the speaker ask the listener to do?</v>
       </c>
       <c r="F31" t="str">
-        <v>A payment schedule</v>
+        <v>Check a catalog.</v>
       </c>
       <c r="G31" t="str">
-        <v>Photographs</v>
+        <v>Send fee information.</v>
       </c>
       <c r="H31" t="str">
-        <v>Shipping information</v>
+        <v>Submit a travel itinerary.</v>
       </c>
       <c r="I31" t="str">
-        <v>Display measurements</v>
+        <v>Update a conference schedule.</v>
       </c>
       <c r="J31" t="str">
-        <v>Câu hỏi về chi tiết, Dạng bài: Telephone message - Tin nhắn thoại</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>